<commit_message>
add side style for cell
</commit_message>
<xml_diff>
--- a/text2.xlsx
+++ b/text2.xlsx
@@ -10,6 +10,248 @@
   </sheets>
   <definedNames/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
+  <si>
+    <t>Унифицированная форма № ТОРГ-12</t>
+  </si>
+  <si>
+    <t>Утверждена постановлением Госкомстата</t>
+  </si>
+  <si>
+    <t>России от 25.12.98 № 132</t>
+  </si>
+  <si>
+    <t>Код</t>
+  </si>
+  <si>
+    <t>Форма по ОКУД</t>
+  </si>
+  <si>
+    <t>0330212</t>
+  </si>
+  <si>
+    <t>по ОКПО</t>
+  </si>
+  <si>
+    <t>(организация-грузоотправитель, адрес, телефон, факс, банковские реквизиты)</t>
+  </si>
+  <si>
+    <t>(структурное подразделение)</t>
+  </si>
+  <si>
+    <t>Вид деятельности по ОКДП</t>
+  </si>
+  <si>
+    <t>Грузополучатель</t>
+  </si>
+  <si>
+    <t>(организация, адрес, телефон, факс, банковские реквизиты)</t>
+  </si>
+  <si>
+    <t>Поставщик</t>
+  </si>
+  <si>
+    <t>Плательщик</t>
+  </si>
+  <si>
+    <t>номер</t>
+  </si>
+  <si>
+    <t>Основание</t>
+  </si>
+  <si>
+    <t>swfidhewfihefiherifhweifhiqwehfliqwhe</t>
+  </si>
+  <si>
+    <t>(договор, заказ-наряд)</t>
+  </si>
+  <si>
+    <t>дата</t>
+  </si>
+  <si>
+    <t>Транспортная накладная</t>
+  </si>
+  <si>
+    <t>Вид операции</t>
+  </si>
+  <si>
+    <t>Номер
+документа</t>
+  </si>
+  <si>
+    <t>Дата
+составления</t>
+  </si>
+  <si>
+    <t>ТОВАРНАЯ НАКЛАДНАЯ</t>
+  </si>
+  <si>
+    <t>Но- мер по по- рядку</t>
+  </si>
+  <si>
+    <t>Товар</t>
+  </si>
+  <si>
+    <t>Единица
+измерения</t>
+  </si>
+  <si>
+    <t>Вид упаков- ки</t>
+  </si>
+  <si>
+    <t>Количество</t>
+  </si>
+  <si>
+    <t>Масса брутто</t>
+  </si>
+  <si>
+    <t>Количест- во
+(масса нетто)</t>
+  </si>
+  <si>
+    <t>Цена,
+руб. коп.</t>
+  </si>
+  <si>
+    <t>Сумма без учета НДС, руб. коп.</t>
+  </si>
+  <si>
+    <t>НДС</t>
+  </si>
+  <si>
+    <t>Сумма с учетом НДС,
+руб. коп.</t>
+  </si>
+  <si>
+    <t>наименование,
+характеристика, сорт, артикул
+товара</t>
+  </si>
+  <si>
+    <t>код</t>
+  </si>
+  <si>
+    <t>наиме- нование</t>
+  </si>
+  <si>
+    <t>код по ОКЕИ</t>
+  </si>
+  <si>
+    <t>в одном месте</t>
+  </si>
+  <si>
+    <t>мест, штук</t>
+  </si>
+  <si>
+    <t>ставка, %</t>
+  </si>
+  <si>
+    <t>сумма,
+руб. коп.</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>asdfnasdkfnlakdsflasdkfnkasdfasdfkoj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   листах</t>
+  </si>
+  <si>
+    <t>и содержит</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   порядковых номеров записей</t>
+  </si>
+  <si>
+    <t>(прописью)</t>
+  </si>
+  <si>
+    <t>Масса груза (нетто)</t>
+  </si>
+  <si>
+    <t>Всего мест</t>
+  </si>
+  <si>
+    <t>Масса груза (брутто)</t>
+  </si>
+  <si>
+    <t>Приложение (паспорта, сертификаты и т.п.) на</t>
+  </si>
+  <si>
+    <t>листах</t>
+  </si>
+  <si>
+    <t>По доверенности №</t>
+  </si>
+  <si>
+    <t>от  «</t>
+  </si>
+  <si>
+    <t>»</t>
+  </si>
+  <si>
+    <t>года,</t>
+  </si>
+  <si>
+    <t>Всего отпущено на сумму</t>
+  </si>
+  <si>
+    <t>выданной</t>
+  </si>
+  <si>
+    <t>(кем, кому (организация, должность, фамилия, и., о.))</t>
+  </si>
+  <si>
+    <t>руб.</t>
+  </si>
+  <si>
+    <t>коп.</t>
+  </si>
+  <si>
+    <t>Отпуск груза разрешил</t>
+  </si>
+  <si>
+    <t>(должность)</t>
+  </si>
+  <si>
+    <t>(подпись)</t>
+  </si>
+  <si>
+    <t>(расшифровка подписи)</t>
+  </si>
+  <si>
+    <t>Главный (старший) бухгалтер</t>
+  </si>
+  <si>
+    <t>Груз принял</t>
+  </si>
+  <si>
+    <t>Отпуск груза произвел</t>
+  </si>
+  <si>
+    <t>Груз получил грузополучатель</t>
+  </si>
+  <si>
+    <t>М.П.</t>
+  </si>
+  <si>
+    <t>«</t>
+  </si>
+  <si>
+    <t>года</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -87,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="72">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -760,182 +1002,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -944,7 +1014,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="116">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1285,41 +1355,12 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="61" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="62" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="42" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="71" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="23" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="70" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="21" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="51" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="24" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="57" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="25" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="26" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="29" fillId="2" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="29" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="64" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="63" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="69" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="66" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="68" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="67" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="34" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="58" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="59" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="43" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="60" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="48" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="49" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="50" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="9" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="53" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="57" fillId="2" fontId="0" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="57" fillId="2" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2406,7 +2447,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="8.83333" defaultRowHeight="12.75" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="8.83333" defaultRowHeight="12.75" outlineLevelCol="0" outlineLevelRow="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="1" width="1.85156"/>
     <col customWidth="1" max="81" min="2" style="1" width="1.67188"/>
@@ -2417,7 +2458,7 @@
     <col customWidth="1" max="256" min="96" style="1" width="8.851559999999999"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="11.25" r="1" s="113">
+    <row customHeight="1" ht="11.25" r="1" s="113" spans="1:95">
       <c r="A1" s="2" t="n"/>
       <c r="B1" s="3" t="n"/>
       <c r="C1" s="3" t="n"/>
@@ -2492,10 +2533,8 @@
       <c r="BT1" s="3" t="n"/>
       <c r="BU1" s="3" t="n"/>
       <c r="BV1" s="3" t="n"/>
-      <c r="BW1" s="4" t="inlineStr">
-        <is>
-          <t>Унифицированная форма № ТОРГ-12</t>
-        </is>
+      <c r="BW1" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="BX1" s="3" t="n"/>
       <c r="BY1" s="3" t="n"/>
@@ -2518,7 +2557,7 @@
       <c r="CP1" s="3" t="n"/>
       <c r="CQ1" s="5" t="n"/>
     </row>
-    <row customHeight="1" ht="10.5" r="2" s="113">
+    <row customHeight="1" ht="10.5" r="2" s="113" spans="1:95">
       <c r="A2" s="6" t="n"/>
       <c r="B2" s="7" t="n"/>
       <c r="C2" s="7" t="n"/>
@@ -2593,10 +2632,8 @@
       <c r="BT2" s="7" t="n"/>
       <c r="BU2" s="7" t="n"/>
       <c r="BV2" s="7" t="n"/>
-      <c r="BW2" s="8" t="inlineStr">
-        <is>
-          <t>Утверждена постановлением Госкомстата</t>
-        </is>
+      <c r="BW2" s="8" t="s">
+        <v>1</v>
       </c>
       <c r="BX2" s="7" t="n"/>
       <c r="BY2" s="7" t="n"/>
@@ -2619,7 +2656,7 @@
       <c r="CP2" s="7" t="n"/>
       <c r="CQ2" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="10.5" r="3" s="113">
+    <row customHeight="1" ht="10.5" r="3" s="113" spans="1:95">
       <c r="A3" s="6" t="n"/>
       <c r="B3" s="7" t="n"/>
       <c r="C3" s="7" t="n"/>
@@ -2694,10 +2731,8 @@
       <c r="BT3" s="7" t="n"/>
       <c r="BU3" s="7" t="n"/>
       <c r="BV3" s="7" t="n"/>
-      <c r="BW3" s="10" t="inlineStr">
-        <is>
-          <t>России от 25.12.98 № 132</t>
-        </is>
+      <c r="BW3" s="10" t="s">
+        <v>2</v>
       </c>
       <c r="BX3" s="7" t="n"/>
       <c r="BY3" s="7" t="n"/>
@@ -2720,7 +2755,7 @@
       <c r="CP3" s="7" t="n"/>
       <c r="CQ3" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="8" r="4" s="113">
+    <row customHeight="1" ht="8" r="4" s="113" spans="1:95">
       <c r="A4" s="6" t="n"/>
       <c r="B4" s="7" t="n"/>
       <c r="C4" s="7" t="n"/>
@@ -2817,7 +2852,7 @@
       <c r="CP4" s="11" t="n"/>
       <c r="CQ4" s="12" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="5" s="113">
+    <row customHeight="1" ht="14.25" r="5" s="113" spans="1:95">
       <c r="A5" s="6" t="n"/>
       <c r="B5" s="7" t="n"/>
       <c r="C5" s="7" t="n"/>
@@ -2901,24 +2936,11 @@
       <c r="CC5" s="7" t="n"/>
       <c r="CD5" s="7" t="n"/>
       <c r="CE5" s="13" t="n"/>
-      <c r="CF5" s="14" t="inlineStr">
-        <is>
-          <t>Код</t>
-        </is>
-      </c>
-      <c r="CG5" s="114" t="n"/>
-      <c r="CH5" s="114" t="n"/>
-      <c r="CI5" s="114" t="n"/>
-      <c r="CJ5" s="114" t="n"/>
-      <c r="CK5" s="114" t="n"/>
-      <c r="CL5" s="114" t="n"/>
-      <c r="CM5" s="114" t="n"/>
-      <c r="CN5" s="114" t="n"/>
-      <c r="CO5" s="114" t="n"/>
-      <c r="CP5" s="114" t="n"/>
-      <c r="CQ5" s="115" t="n"/>
+      <c r="CF5" s="14" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row customHeight="1" ht="15.75" r="6" s="113">
+    <row customHeight="1" ht="15.75" r="6" s="113" spans="1:95">
       <c r="A6" s="6" t="n"/>
       <c r="B6" s="7" t="n"/>
       <c r="C6" s="7" t="n"/>
@@ -3000,201 +3022,31 @@
       <c r="CA6" s="7" t="n"/>
       <c r="CB6" s="7" t="n"/>
       <c r="CC6" s="7" t="n"/>
-      <c r="CD6" s="16" t="inlineStr">
-        <is>
-          <t>Форма по ОКУД</t>
-        </is>
+      <c r="CD6" s="16" t="s">
+        <v>4</v>
       </c>
       <c r="CE6" s="17" t="n"/>
-      <c r="CF6" s="18" t="inlineStr">
-        <is>
-          <t>0330212</t>
-        </is>
-      </c>
-      <c r="CG6" s="116" t="n"/>
-      <c r="CH6" s="116" t="n"/>
-      <c r="CI6" s="116" t="n"/>
-      <c r="CJ6" s="116" t="n"/>
-      <c r="CK6" s="116" t="n"/>
-      <c r="CL6" s="116" t="n"/>
-      <c r="CM6" s="116" t="n"/>
-      <c r="CN6" s="116" t="n"/>
-      <c r="CO6" s="116" t="n"/>
-      <c r="CP6" s="116" t="n"/>
-      <c r="CQ6" s="117" t="n"/>
+      <c r="CF6" s="18" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row customHeight="1" ht="15.75" r="7" s="113">
+    <row customHeight="1" ht="15.75" r="7" s="113" spans="1:95">
       <c r="A7" s="20" t="n"/>
-      <c r="B7" s="118" t="n"/>
-      <c r="C7" s="118" t="n"/>
-      <c r="D7" s="118" t="n"/>
-      <c r="E7" s="118" t="n"/>
-      <c r="F7" s="118" t="n"/>
-      <c r="G7" s="118" t="n"/>
-      <c r="H7" s="118" t="n"/>
-      <c r="I7" s="118" t="n"/>
-      <c r="J7" s="118" t="n"/>
-      <c r="K7" s="118" t="n"/>
-      <c r="L7" s="118" t="n"/>
-      <c r="M7" s="118" t="n"/>
-      <c r="N7" s="118" t="n"/>
-      <c r="O7" s="118" t="n"/>
-      <c r="P7" s="118" t="n"/>
-      <c r="Q7" s="118" t="n"/>
-      <c r="R7" s="118" t="n"/>
-      <c r="S7" s="118" t="n"/>
-      <c r="T7" s="118" t="n"/>
-      <c r="U7" s="118" t="n"/>
-      <c r="V7" s="118" t="n"/>
-      <c r="W7" s="118" t="n"/>
-      <c r="X7" s="118" t="n"/>
-      <c r="Y7" s="118" t="n"/>
-      <c r="Z7" s="118" t="n"/>
-      <c r="AA7" s="118" t="n"/>
-      <c r="AB7" s="118" t="n"/>
-      <c r="AC7" s="118" t="n"/>
-      <c r="AD7" s="118" t="n"/>
-      <c r="AE7" s="118" t="n"/>
-      <c r="AF7" s="118" t="n"/>
-      <c r="AG7" s="118" t="n"/>
-      <c r="AH7" s="118" t="n"/>
-      <c r="AI7" s="118" t="n"/>
-      <c r="AJ7" s="118" t="n"/>
-      <c r="AK7" s="118" t="n"/>
-      <c r="AL7" s="118" t="n"/>
-      <c r="AM7" s="118" t="n"/>
-      <c r="AN7" s="118" t="n"/>
-      <c r="AO7" s="118" t="n"/>
-      <c r="AP7" s="118" t="n"/>
-      <c r="AQ7" s="118" t="n"/>
-      <c r="AR7" s="118" t="n"/>
-      <c r="AS7" s="118" t="n"/>
-      <c r="AT7" s="118" t="n"/>
-      <c r="AU7" s="118" t="n"/>
-      <c r="AV7" s="118" t="n"/>
-      <c r="AW7" s="118" t="n"/>
-      <c r="AX7" s="118" t="n"/>
-      <c r="AY7" s="118" t="n"/>
-      <c r="AZ7" s="118" t="n"/>
-      <c r="BA7" s="118" t="n"/>
-      <c r="BB7" s="118" t="n"/>
-      <c r="BC7" s="118" t="n"/>
-      <c r="BD7" s="118" t="n"/>
-      <c r="BE7" s="118" t="n"/>
-      <c r="BF7" s="118" t="n"/>
-      <c r="BG7" s="118" t="n"/>
-      <c r="BH7" s="118" t="n"/>
-      <c r="BI7" s="118" t="n"/>
-      <c r="BJ7" s="118" t="n"/>
-      <c r="BK7" s="118" t="n"/>
-      <c r="BL7" s="118" t="n"/>
-      <c r="BM7" s="118" t="n"/>
-      <c r="BN7" s="118" t="n"/>
-      <c r="BO7" s="118" t="n"/>
-      <c r="BP7" s="118" t="n"/>
-      <c r="BQ7" s="118" t="n"/>
-      <c r="BR7" s="118" t="n"/>
-      <c r="BS7" s="118" t="n"/>
-      <c r="BT7" s="118" t="n"/>
-      <c r="BU7" s="118" t="n"/>
-      <c r="BV7" s="118" t="n"/>
-      <c r="BW7" s="118" t="n"/>
-      <c r="BX7" s="119" t="n"/>
       <c r="BY7" s="7" t="n"/>
       <c r="BZ7" s="7" t="n"/>
       <c r="CA7" s="7" t="n"/>
       <c r="CB7" s="7" t="n"/>
       <c r="CC7" s="7" t="n"/>
-      <c r="CD7" s="16" t="inlineStr">
-        <is>
-          <t>по ОКПО</t>
-        </is>
+      <c r="CD7" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="CE7" s="17" t="n"/>
       <c r="CF7" s="22" t="n"/>
-      <c r="CG7" s="120" t="n"/>
-      <c r="CH7" s="120" t="n"/>
-      <c r="CI7" s="120" t="n"/>
-      <c r="CJ7" s="120" t="n"/>
-      <c r="CK7" s="120" t="n"/>
-      <c r="CL7" s="120" t="n"/>
-      <c r="CM7" s="120" t="n"/>
-      <c r="CN7" s="120" t="n"/>
-      <c r="CO7" s="120" t="n"/>
-      <c r="CP7" s="120" t="n"/>
-      <c r="CQ7" s="121" t="n"/>
     </row>
-    <row customHeight="1" ht="8.25" r="8" s="113">
-      <c r="A8" s="24" t="inlineStr">
-        <is>
-          <t>(организация-грузоотправитель, адрес, телефон, факс, банковские реквизиты)</t>
-        </is>
-      </c>
-      <c r="B8" s="122" t="n"/>
-      <c r="C8" s="122" t="n"/>
-      <c r="D8" s="122" t="n"/>
-      <c r="E8" s="122" t="n"/>
-      <c r="F8" s="122" t="n"/>
-      <c r="G8" s="122" t="n"/>
-      <c r="H8" s="122" t="n"/>
-      <c r="I8" s="122" t="n"/>
-      <c r="J8" s="122" t="n"/>
-      <c r="K8" s="122" t="n"/>
-      <c r="L8" s="122" t="n"/>
-      <c r="M8" s="122" t="n"/>
-      <c r="N8" s="122" t="n"/>
-      <c r="O8" s="122" t="n"/>
-      <c r="P8" s="122" t="n"/>
-      <c r="Q8" s="122" t="n"/>
-      <c r="R8" s="122" t="n"/>
-      <c r="S8" s="122" t="n"/>
-      <c r="T8" s="122" t="n"/>
-      <c r="U8" s="122" t="n"/>
-      <c r="V8" s="122" t="n"/>
-      <c r="W8" s="122" t="n"/>
-      <c r="X8" s="122" t="n"/>
-      <c r="Y8" s="122" t="n"/>
-      <c r="Z8" s="122" t="n"/>
-      <c r="AA8" s="122" t="n"/>
-      <c r="AB8" s="122" t="n"/>
-      <c r="AC8" s="122" t="n"/>
-      <c r="AD8" s="122" t="n"/>
-      <c r="AE8" s="122" t="n"/>
-      <c r="AF8" s="122" t="n"/>
-      <c r="AG8" s="122" t="n"/>
-      <c r="AH8" s="122" t="n"/>
-      <c r="AI8" s="122" t="n"/>
-      <c r="AJ8" s="122" t="n"/>
-      <c r="AK8" s="122" t="n"/>
-      <c r="AL8" s="122" t="n"/>
-      <c r="AM8" s="122" t="n"/>
-      <c r="AN8" s="122" t="n"/>
-      <c r="AO8" s="122" t="n"/>
-      <c r="AP8" s="122" t="n"/>
-      <c r="AQ8" s="122" t="n"/>
-      <c r="AR8" s="122" t="n"/>
-      <c r="AS8" s="122" t="n"/>
-      <c r="AT8" s="122" t="n"/>
-      <c r="AU8" s="122" t="n"/>
-      <c r="AV8" s="122" t="n"/>
-      <c r="AW8" s="122" t="n"/>
-      <c r="AX8" s="122" t="n"/>
-      <c r="AY8" s="122" t="n"/>
-      <c r="AZ8" s="122" t="n"/>
-      <c r="BA8" s="122" t="n"/>
-      <c r="BB8" s="122" t="n"/>
-      <c r="BC8" s="122" t="n"/>
-      <c r="BD8" s="122" t="n"/>
-      <c r="BE8" s="122" t="n"/>
-      <c r="BF8" s="122" t="n"/>
-      <c r="BG8" s="122" t="n"/>
-      <c r="BH8" s="122" t="n"/>
-      <c r="BI8" s="122" t="n"/>
-      <c r="BJ8" s="122" t="n"/>
-      <c r="BK8" s="122" t="n"/>
-      <c r="BL8" s="122" t="n"/>
-      <c r="BM8" s="122" t="n"/>
-      <c r="BN8" s="123" t="n"/>
+    <row customHeight="1" ht="8.25" r="8" s="113" spans="1:95">
+      <c r="A8" s="24" t="s">
+        <v>7</v>
+      </c>
       <c r="BO8" s="26" t="n"/>
       <c r="BP8" s="26" t="n"/>
       <c r="BQ8" s="26" t="n"/>
@@ -3213,221 +3065,21 @@
       <c r="CD8" s="27" t="n"/>
       <c r="CE8" s="17" t="n"/>
       <c r="CF8" s="22" t="n"/>
-      <c r="CG8" s="122" t="n"/>
-      <c r="CH8" s="122" t="n"/>
-      <c r="CI8" s="122" t="n"/>
-      <c r="CJ8" s="122" t="n"/>
-      <c r="CK8" s="122" t="n"/>
-      <c r="CL8" s="122" t="n"/>
-      <c r="CM8" s="122" t="n"/>
-      <c r="CN8" s="122" t="n"/>
-      <c r="CO8" s="122" t="n"/>
-      <c r="CP8" s="122" t="n"/>
-      <c r="CQ8" s="124" t="n"/>
     </row>
-    <row customHeight="1" ht="10.5" r="9" s="113">
+    <row customHeight="1" ht="10.5" r="9" s="113" spans="1:95">
       <c r="A9" s="20" t="n"/>
-      <c r="B9" s="118" t="n"/>
-      <c r="C9" s="118" t="n"/>
-      <c r="D9" s="118" t="n"/>
-      <c r="E9" s="118" t="n"/>
-      <c r="F9" s="118" t="n"/>
-      <c r="G9" s="118" t="n"/>
-      <c r="H9" s="118" t="n"/>
-      <c r="I9" s="118" t="n"/>
-      <c r="J9" s="118" t="n"/>
-      <c r="K9" s="118" t="n"/>
-      <c r="L9" s="118" t="n"/>
-      <c r="M9" s="118" t="n"/>
-      <c r="N9" s="118" t="n"/>
-      <c r="O9" s="118" t="n"/>
-      <c r="P9" s="118" t="n"/>
-      <c r="Q9" s="118" t="n"/>
-      <c r="R9" s="118" t="n"/>
-      <c r="S9" s="118" t="n"/>
-      <c r="T9" s="118" t="n"/>
-      <c r="U9" s="118" t="n"/>
-      <c r="V9" s="118" t="n"/>
-      <c r="W9" s="118" t="n"/>
-      <c r="X9" s="118" t="n"/>
-      <c r="Y9" s="118" t="n"/>
-      <c r="Z9" s="118" t="n"/>
-      <c r="AA9" s="118" t="n"/>
-      <c r="AB9" s="118" t="n"/>
-      <c r="AC9" s="118" t="n"/>
-      <c r="AD9" s="118" t="n"/>
-      <c r="AE9" s="118" t="n"/>
-      <c r="AF9" s="118" t="n"/>
-      <c r="AG9" s="118" t="n"/>
-      <c r="AH9" s="118" t="n"/>
-      <c r="AI9" s="118" t="n"/>
-      <c r="AJ9" s="118" t="n"/>
-      <c r="AK9" s="118" t="n"/>
-      <c r="AL9" s="118" t="n"/>
-      <c r="AM9" s="118" t="n"/>
-      <c r="AN9" s="118" t="n"/>
-      <c r="AO9" s="118" t="n"/>
-      <c r="AP9" s="118" t="n"/>
-      <c r="AQ9" s="118" t="n"/>
-      <c r="AR9" s="118" t="n"/>
-      <c r="AS9" s="118" t="n"/>
-      <c r="AT9" s="118" t="n"/>
-      <c r="AU9" s="118" t="n"/>
-      <c r="AV9" s="118" t="n"/>
-      <c r="AW9" s="118" t="n"/>
-      <c r="AX9" s="118" t="n"/>
-      <c r="AY9" s="118" t="n"/>
-      <c r="AZ9" s="118" t="n"/>
-      <c r="BA9" s="118" t="n"/>
-      <c r="BB9" s="118" t="n"/>
-      <c r="BC9" s="118" t="n"/>
-      <c r="BD9" s="118" t="n"/>
-      <c r="BE9" s="118" t="n"/>
-      <c r="BF9" s="118" t="n"/>
-      <c r="BG9" s="118" t="n"/>
-      <c r="BH9" s="118" t="n"/>
-      <c r="BI9" s="118" t="n"/>
-      <c r="BJ9" s="118" t="n"/>
-      <c r="BK9" s="118" t="n"/>
-      <c r="BL9" s="118" t="n"/>
-      <c r="BM9" s="118" t="n"/>
-      <c r="BN9" s="118" t="n"/>
-      <c r="BO9" s="118" t="n"/>
-      <c r="BP9" s="118" t="n"/>
-      <c r="BQ9" s="118" t="n"/>
-      <c r="BR9" s="118" t="n"/>
-      <c r="BS9" s="118" t="n"/>
-      <c r="BT9" s="118" t="n"/>
-      <c r="BU9" s="118" t="n"/>
-      <c r="BV9" s="118" t="n"/>
-      <c r="BW9" s="118" t="n"/>
-      <c r="BX9" s="118" t="n"/>
-      <c r="BY9" s="118" t="n"/>
-      <c r="BZ9" s="118" t="n"/>
-      <c r="CA9" s="118" t="n"/>
-      <c r="CB9" s="118" t="n"/>
-      <c r="CC9" s="118" t="n"/>
-      <c r="CD9" s="118" t="n"/>
-      <c r="CE9" s="119" t="n"/>
-      <c r="CF9" s="125" t="n"/>
-      <c r="CG9" s="118" t="n"/>
-      <c r="CH9" s="118" t="n"/>
-      <c r="CI9" s="118" t="n"/>
-      <c r="CJ9" s="118" t="n"/>
-      <c r="CK9" s="118" t="n"/>
-      <c r="CL9" s="118" t="n"/>
-      <c r="CM9" s="118" t="n"/>
-      <c r="CN9" s="118" t="n"/>
-      <c r="CO9" s="118" t="n"/>
-      <c r="CP9" s="118" t="n"/>
-      <c r="CQ9" s="126" t="n"/>
     </row>
-    <row customHeight="1" ht="8" r="10" s="113">
-      <c r="A10" s="24" t="inlineStr">
-        <is>
-          <t>(структурное подразделение)</t>
-        </is>
-      </c>
-      <c r="B10" s="122" t="n"/>
-      <c r="C10" s="122" t="n"/>
-      <c r="D10" s="122" t="n"/>
-      <c r="E10" s="122" t="n"/>
-      <c r="F10" s="122" t="n"/>
-      <c r="G10" s="122" t="n"/>
-      <c r="H10" s="122" t="n"/>
-      <c r="I10" s="122" t="n"/>
-      <c r="J10" s="122" t="n"/>
-      <c r="K10" s="122" t="n"/>
-      <c r="L10" s="122" t="n"/>
-      <c r="M10" s="122" t="n"/>
-      <c r="N10" s="122" t="n"/>
-      <c r="O10" s="122" t="n"/>
-      <c r="P10" s="122" t="n"/>
-      <c r="Q10" s="122" t="n"/>
-      <c r="R10" s="122" t="n"/>
-      <c r="S10" s="122" t="n"/>
-      <c r="T10" s="122" t="n"/>
-      <c r="U10" s="122" t="n"/>
-      <c r="V10" s="122" t="n"/>
-      <c r="W10" s="122" t="n"/>
-      <c r="X10" s="122" t="n"/>
-      <c r="Y10" s="122" t="n"/>
-      <c r="Z10" s="122" t="n"/>
-      <c r="AA10" s="122" t="n"/>
-      <c r="AB10" s="122" t="n"/>
-      <c r="AC10" s="122" t="n"/>
-      <c r="AD10" s="122" t="n"/>
-      <c r="AE10" s="122" t="n"/>
-      <c r="AF10" s="122" t="n"/>
-      <c r="AG10" s="122" t="n"/>
-      <c r="AH10" s="122" t="n"/>
-      <c r="AI10" s="122" t="n"/>
-      <c r="AJ10" s="122" t="n"/>
-      <c r="AK10" s="122" t="n"/>
-      <c r="AL10" s="122" t="n"/>
-      <c r="AM10" s="122" t="n"/>
-      <c r="AN10" s="122" t="n"/>
-      <c r="AO10" s="122" t="n"/>
-      <c r="AP10" s="122" t="n"/>
-      <c r="AQ10" s="122" t="n"/>
-      <c r="AR10" s="122" t="n"/>
-      <c r="AS10" s="122" t="n"/>
-      <c r="AT10" s="122" t="n"/>
-      <c r="AU10" s="122" t="n"/>
-      <c r="AV10" s="122" t="n"/>
-      <c r="AW10" s="122" t="n"/>
-      <c r="AX10" s="122" t="n"/>
-      <c r="AY10" s="122" t="n"/>
-      <c r="AZ10" s="122" t="n"/>
-      <c r="BA10" s="122" t="n"/>
-      <c r="BB10" s="122" t="n"/>
-      <c r="BC10" s="122" t="n"/>
-      <c r="BD10" s="122" t="n"/>
-      <c r="BE10" s="122" t="n"/>
-      <c r="BF10" s="122" t="n"/>
-      <c r="BG10" s="122" t="n"/>
-      <c r="BH10" s="122" t="n"/>
-      <c r="BI10" s="122" t="n"/>
-      <c r="BJ10" s="122" t="n"/>
-      <c r="BK10" s="122" t="n"/>
-      <c r="BL10" s="122" t="n"/>
-      <c r="BM10" s="122" t="n"/>
-      <c r="BN10" s="123" t="n"/>
-      <c r="BO10" s="29" t="inlineStr">
-        <is>
-          <t>Вид деятельности по ОКДП</t>
-        </is>
-      </c>
-      <c r="BP10" s="122" t="n"/>
-      <c r="BQ10" s="122" t="n"/>
-      <c r="BR10" s="122" t="n"/>
-      <c r="BS10" s="122" t="n"/>
-      <c r="BT10" s="122" t="n"/>
-      <c r="BU10" s="122" t="n"/>
-      <c r="BV10" s="122" t="n"/>
-      <c r="BW10" s="122" t="n"/>
-      <c r="BX10" s="122" t="n"/>
-      <c r="BY10" s="122" t="n"/>
-      <c r="BZ10" s="122" t="n"/>
-      <c r="CA10" s="122" t="n"/>
-      <c r="CB10" s="122" t="n"/>
-      <c r="CC10" s="122" t="n"/>
-      <c r="CD10" s="122" t="n"/>
+    <row customHeight="1" ht="8" r="10" s="113" spans="1:95">
+      <c r="A10" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BO10" s="29" t="s">
+        <v>9</v>
+      </c>
       <c r="CE10" s="30" t="n"/>
       <c r="CF10" s="22" t="n"/>
-      <c r="CG10" s="122" t="n"/>
-      <c r="CH10" s="122" t="n"/>
-      <c r="CI10" s="122" t="n"/>
-      <c r="CJ10" s="122" t="n"/>
-      <c r="CK10" s="122" t="n"/>
-      <c r="CL10" s="122" t="n"/>
-      <c r="CM10" s="122" t="n"/>
-      <c r="CN10" s="122" t="n"/>
-      <c r="CO10" s="122" t="n"/>
-      <c r="CP10" s="122" t="n"/>
-      <c r="CQ10" s="124" t="n"/>
     </row>
-    <row customHeight="1" ht="9" r="11" s="113">
+    <row customHeight="1" ht="9" r="11" s="113" spans="1:95">
       <c r="A11" s="6" t="n"/>
       <c r="B11" s="7" t="n"/>
       <c r="C11" s="7" t="n"/>
@@ -3494,42 +3146,12 @@
       <c r="BL11" s="7" t="n"/>
       <c r="BM11" s="7" t="n"/>
       <c r="BN11" s="7" t="n"/>
-      <c r="BO11" s="118" t="n"/>
-      <c r="BP11" s="118" t="n"/>
-      <c r="BQ11" s="118" t="n"/>
-      <c r="BR11" s="118" t="n"/>
-      <c r="BS11" s="118" t="n"/>
-      <c r="BT11" s="118" t="n"/>
-      <c r="BU11" s="118" t="n"/>
-      <c r="BV11" s="118" t="n"/>
-      <c r="BW11" s="118" t="n"/>
-      <c r="BX11" s="118" t="n"/>
-      <c r="BY11" s="118" t="n"/>
-      <c r="BZ11" s="118" t="n"/>
-      <c r="CA11" s="118" t="n"/>
-      <c r="CB11" s="118" t="n"/>
-      <c r="CC11" s="118" t="n"/>
-      <c r="CD11" s="118" t="n"/>
       <c r="CE11" s="17" t="n"/>
-      <c r="CF11" s="125" t="n"/>
-      <c r="CG11" s="118" t="n"/>
-      <c r="CH11" s="118" t="n"/>
-      <c r="CI11" s="118" t="n"/>
-      <c r="CJ11" s="118" t="n"/>
-      <c r="CK11" s="118" t="n"/>
-      <c r="CL11" s="118" t="n"/>
-      <c r="CM11" s="118" t="n"/>
-      <c r="CN11" s="118" t="n"/>
-      <c r="CO11" s="118" t="n"/>
-      <c r="CP11" s="118" t="n"/>
-      <c r="CQ11" s="126" t="n"/>
     </row>
-    <row customHeight="1" ht="17.25" r="12" s="113">
+    <row customHeight="1" ht="17.25" r="12" s="113" spans="1:95">
       <c r="A12" s="6" t="n"/>
-      <c r="B12" s="32" t="inlineStr">
-        <is>
-          <t>Грузополучатель</t>
-        </is>
+      <c r="B12" s="32" t="s">
+        <v>10</v>
       </c>
       <c r="C12" s="7" t="n"/>
       <c r="D12" s="7" t="n"/>
@@ -3541,95 +3163,18 @@
       <c r="J12" s="7" t="n"/>
       <c r="K12" s="7" t="n"/>
       <c r="L12" s="33" t="n"/>
-      <c r="M12" s="118" t="n"/>
-      <c r="N12" s="118" t="n"/>
-      <c r="O12" s="118" t="n"/>
-      <c r="P12" s="118" t="n"/>
-      <c r="Q12" s="118" t="n"/>
-      <c r="R12" s="118" t="n"/>
-      <c r="S12" s="118" t="n"/>
-      <c r="T12" s="118" t="n"/>
-      <c r="U12" s="118" t="n"/>
-      <c r="V12" s="118" t="n"/>
-      <c r="W12" s="118" t="n"/>
-      <c r="X12" s="118" t="n"/>
-      <c r="Y12" s="118" t="n"/>
-      <c r="Z12" s="118" t="n"/>
-      <c r="AA12" s="118" t="n"/>
-      <c r="AB12" s="118" t="n"/>
-      <c r="AC12" s="118" t="n"/>
-      <c r="AD12" s="118" t="n"/>
-      <c r="AE12" s="118" t="n"/>
-      <c r="AF12" s="118" t="n"/>
-      <c r="AG12" s="118" t="n"/>
-      <c r="AH12" s="118" t="n"/>
-      <c r="AI12" s="118" t="n"/>
-      <c r="AJ12" s="118" t="n"/>
-      <c r="AK12" s="118" t="n"/>
-      <c r="AL12" s="118" t="n"/>
-      <c r="AM12" s="118" t="n"/>
-      <c r="AN12" s="118" t="n"/>
-      <c r="AO12" s="118" t="n"/>
-      <c r="AP12" s="118" t="n"/>
-      <c r="AQ12" s="118" t="n"/>
-      <c r="AR12" s="118" t="n"/>
-      <c r="AS12" s="118" t="n"/>
-      <c r="AT12" s="118" t="n"/>
-      <c r="AU12" s="118" t="n"/>
-      <c r="AV12" s="118" t="n"/>
-      <c r="AW12" s="118" t="n"/>
-      <c r="AX12" s="118" t="n"/>
-      <c r="AY12" s="118" t="n"/>
-      <c r="AZ12" s="118" t="n"/>
-      <c r="BA12" s="118" t="n"/>
-      <c r="BB12" s="118" t="n"/>
-      <c r="BC12" s="118" t="n"/>
-      <c r="BD12" s="118" t="n"/>
-      <c r="BE12" s="118" t="n"/>
-      <c r="BF12" s="118" t="n"/>
-      <c r="BG12" s="118" t="n"/>
-      <c r="BH12" s="118" t="n"/>
-      <c r="BI12" s="118" t="n"/>
-      <c r="BJ12" s="118" t="n"/>
-      <c r="BK12" s="118" t="n"/>
-      <c r="BL12" s="118" t="n"/>
-      <c r="BM12" s="118" t="n"/>
-      <c r="BN12" s="118" t="n"/>
-      <c r="BO12" s="118" t="n"/>
-      <c r="BP12" s="118" t="n"/>
-      <c r="BQ12" s="118" t="n"/>
-      <c r="BR12" s="118" t="n"/>
-      <c r="BS12" s="118" t="n"/>
-      <c r="BT12" s="118" t="n"/>
-      <c r="BU12" s="118" t="n"/>
-      <c r="BV12" s="118" t="n"/>
-      <c r="BW12" s="118" t="n"/>
-      <c r="BX12" s="118" t="n"/>
       <c r="BY12" s="34" t="n"/>
       <c r="BZ12" s="34" t="n"/>
       <c r="CA12" s="34" t="n"/>
       <c r="CB12" s="34" t="n"/>
       <c r="CC12" s="34" t="n"/>
-      <c r="CD12" s="16" t="inlineStr">
-        <is>
-          <t>по ОКПО</t>
-        </is>
+      <c r="CD12" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="CE12" s="17" t="n"/>
       <c r="CF12" s="22" t="n"/>
-      <c r="CG12" s="120" t="n"/>
-      <c r="CH12" s="120" t="n"/>
-      <c r="CI12" s="120" t="n"/>
-      <c r="CJ12" s="120" t="n"/>
-      <c r="CK12" s="120" t="n"/>
-      <c r="CL12" s="120" t="n"/>
-      <c r="CM12" s="120" t="n"/>
-      <c r="CN12" s="120" t="n"/>
-      <c r="CO12" s="120" t="n"/>
-      <c r="CP12" s="120" t="n"/>
-      <c r="CQ12" s="121" t="n"/>
     </row>
-    <row customHeight="1" ht="8.25" r="13" s="113">
+    <row customHeight="1" ht="8.25" r="13" s="113" spans="1:95">
       <c r="A13" s="6" t="n"/>
       <c r="B13" s="34" t="n"/>
       <c r="C13" s="7" t="n"/>
@@ -3641,75 +3186,9 @@
       <c r="I13" s="7" t="n"/>
       <c r="J13" s="7" t="n"/>
       <c r="K13" s="7" t="n"/>
-      <c r="L13" s="35" t="inlineStr">
-        <is>
-          <t>(организация, адрес, телефон, факс, банковские реквизиты)</t>
-        </is>
-      </c>
-      <c r="M13" s="122" t="n"/>
-      <c r="N13" s="122" t="n"/>
-      <c r="O13" s="122" t="n"/>
-      <c r="P13" s="122" t="n"/>
-      <c r="Q13" s="122" t="n"/>
-      <c r="R13" s="122" t="n"/>
-      <c r="S13" s="122" t="n"/>
-      <c r="T13" s="122" t="n"/>
-      <c r="U13" s="122" t="n"/>
-      <c r="V13" s="122" t="n"/>
-      <c r="W13" s="122" t="n"/>
-      <c r="X13" s="122" t="n"/>
-      <c r="Y13" s="122" t="n"/>
-      <c r="Z13" s="122" t="n"/>
-      <c r="AA13" s="122" t="n"/>
-      <c r="AB13" s="122" t="n"/>
-      <c r="AC13" s="122" t="n"/>
-      <c r="AD13" s="122" t="n"/>
-      <c r="AE13" s="122" t="n"/>
-      <c r="AF13" s="122" t="n"/>
-      <c r="AG13" s="122" t="n"/>
-      <c r="AH13" s="122" t="n"/>
-      <c r="AI13" s="122" t="n"/>
-      <c r="AJ13" s="122" t="n"/>
-      <c r="AK13" s="122" t="n"/>
-      <c r="AL13" s="122" t="n"/>
-      <c r="AM13" s="122" t="n"/>
-      <c r="AN13" s="122" t="n"/>
-      <c r="AO13" s="122" t="n"/>
-      <c r="AP13" s="122" t="n"/>
-      <c r="AQ13" s="122" t="n"/>
-      <c r="AR13" s="122" t="n"/>
-      <c r="AS13" s="122" t="n"/>
-      <c r="AT13" s="122" t="n"/>
-      <c r="AU13" s="122" t="n"/>
-      <c r="AV13" s="122" t="n"/>
-      <c r="AW13" s="122" t="n"/>
-      <c r="AX13" s="122" t="n"/>
-      <c r="AY13" s="122" t="n"/>
-      <c r="AZ13" s="122" t="n"/>
-      <c r="BA13" s="122" t="n"/>
-      <c r="BB13" s="122" t="n"/>
-      <c r="BC13" s="122" t="n"/>
-      <c r="BD13" s="122" t="n"/>
-      <c r="BE13" s="122" t="n"/>
-      <c r="BF13" s="122" t="n"/>
-      <c r="BG13" s="122" t="n"/>
-      <c r="BH13" s="122" t="n"/>
-      <c r="BI13" s="122" t="n"/>
-      <c r="BJ13" s="122" t="n"/>
-      <c r="BK13" s="122" t="n"/>
-      <c r="BL13" s="122" t="n"/>
-      <c r="BM13" s="122" t="n"/>
-      <c r="BN13" s="122" t="n"/>
-      <c r="BO13" s="122" t="n"/>
-      <c r="BP13" s="122" t="n"/>
-      <c r="BQ13" s="122" t="n"/>
-      <c r="BR13" s="122" t="n"/>
-      <c r="BS13" s="122" t="n"/>
-      <c r="BT13" s="122" t="n"/>
-      <c r="BU13" s="122" t="n"/>
-      <c r="BV13" s="122" t="n"/>
-      <c r="BW13" s="122" t="n"/>
-      <c r="BX13" s="122" t="n"/>
+      <c r="L13" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="BY13" s="34" t="n"/>
       <c r="BZ13" s="34" t="n"/>
       <c r="CA13" s="34" t="n"/>
@@ -3718,24 +3197,11 @@
       <c r="CD13" s="36" t="n"/>
       <c r="CE13" s="17" t="n"/>
       <c r="CF13" s="22" t="n"/>
-      <c r="CG13" s="122" t="n"/>
-      <c r="CH13" s="122" t="n"/>
-      <c r="CI13" s="122" t="n"/>
-      <c r="CJ13" s="122" t="n"/>
-      <c r="CK13" s="122" t="n"/>
-      <c r="CL13" s="122" t="n"/>
-      <c r="CM13" s="122" t="n"/>
-      <c r="CN13" s="122" t="n"/>
-      <c r="CO13" s="122" t="n"/>
-      <c r="CP13" s="122" t="n"/>
-      <c r="CQ13" s="124" t="n"/>
     </row>
-    <row customHeight="1" ht="11.25" r="14" s="113">
+    <row customHeight="1" ht="11.25" r="14" s="113" spans="1:95">
       <c r="A14" s="6" t="n"/>
-      <c r="B14" s="32" t="inlineStr">
-        <is>
-          <t>Поставщик</t>
-        </is>
+      <c r="B14" s="32" t="s">
+        <v>12</v>
       </c>
       <c r="C14" s="7" t="n"/>
       <c r="D14" s="7" t="n"/>
@@ -3744,98 +3210,17 @@
       <c r="G14" s="7" t="n"/>
       <c r="H14" s="7" t="n"/>
       <c r="I14" s="33" t="n"/>
-      <c r="J14" s="118" t="n"/>
-      <c r="K14" s="118" t="n"/>
-      <c r="L14" s="118" t="n"/>
-      <c r="M14" s="118" t="n"/>
-      <c r="N14" s="118" t="n"/>
-      <c r="O14" s="118" t="n"/>
-      <c r="P14" s="118" t="n"/>
-      <c r="Q14" s="118" t="n"/>
-      <c r="R14" s="118" t="n"/>
-      <c r="S14" s="118" t="n"/>
-      <c r="T14" s="118" t="n"/>
-      <c r="U14" s="118" t="n"/>
-      <c r="V14" s="118" t="n"/>
-      <c r="W14" s="118" t="n"/>
-      <c r="X14" s="118" t="n"/>
-      <c r="Y14" s="118" t="n"/>
-      <c r="Z14" s="118" t="n"/>
-      <c r="AA14" s="118" t="n"/>
-      <c r="AB14" s="118" t="n"/>
-      <c r="AC14" s="118" t="n"/>
-      <c r="AD14" s="118" t="n"/>
-      <c r="AE14" s="118" t="n"/>
-      <c r="AF14" s="118" t="n"/>
-      <c r="AG14" s="118" t="n"/>
-      <c r="AH14" s="118" t="n"/>
-      <c r="AI14" s="118" t="n"/>
-      <c r="AJ14" s="118" t="n"/>
-      <c r="AK14" s="118" t="n"/>
-      <c r="AL14" s="118" t="n"/>
-      <c r="AM14" s="118" t="n"/>
-      <c r="AN14" s="118" t="n"/>
-      <c r="AO14" s="118" t="n"/>
-      <c r="AP14" s="118" t="n"/>
-      <c r="AQ14" s="118" t="n"/>
-      <c r="AR14" s="118" t="n"/>
-      <c r="AS14" s="118" t="n"/>
-      <c r="AT14" s="118" t="n"/>
-      <c r="AU14" s="118" t="n"/>
-      <c r="AV14" s="118" t="n"/>
-      <c r="AW14" s="118" t="n"/>
-      <c r="AX14" s="118" t="n"/>
-      <c r="AY14" s="118" t="n"/>
-      <c r="AZ14" s="118" t="n"/>
-      <c r="BA14" s="118" t="n"/>
-      <c r="BB14" s="118" t="n"/>
-      <c r="BC14" s="118" t="n"/>
-      <c r="BD14" s="118" t="n"/>
-      <c r="BE14" s="118" t="n"/>
-      <c r="BF14" s="118" t="n"/>
-      <c r="BG14" s="118" t="n"/>
-      <c r="BH14" s="118" t="n"/>
-      <c r="BI14" s="118" t="n"/>
-      <c r="BJ14" s="118" t="n"/>
-      <c r="BK14" s="118" t="n"/>
-      <c r="BL14" s="118" t="n"/>
-      <c r="BM14" s="118" t="n"/>
-      <c r="BN14" s="118" t="n"/>
-      <c r="BO14" s="118" t="n"/>
-      <c r="BP14" s="118" t="n"/>
-      <c r="BQ14" s="118" t="n"/>
-      <c r="BR14" s="118" t="n"/>
-      <c r="BS14" s="118" t="n"/>
-      <c r="BT14" s="118" t="n"/>
-      <c r="BU14" s="118" t="n"/>
-      <c r="BV14" s="118" t="n"/>
-      <c r="BW14" s="118" t="n"/>
-      <c r="BX14" s="118" t="n"/>
       <c r="BY14" s="34" t="n"/>
       <c r="BZ14" s="34" t="n"/>
       <c r="CA14" s="34" t="n"/>
       <c r="CB14" s="34" t="n"/>
       <c r="CC14" s="34" t="n"/>
-      <c r="CD14" s="16" t="inlineStr">
-        <is>
-          <t>по ОКПО</t>
-        </is>
+      <c r="CD14" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="CE14" s="17" t="n"/>
-      <c r="CF14" s="125" t="n"/>
-      <c r="CG14" s="118" t="n"/>
-      <c r="CH14" s="118" t="n"/>
-      <c r="CI14" s="118" t="n"/>
-      <c r="CJ14" s="118" t="n"/>
-      <c r="CK14" s="118" t="n"/>
-      <c r="CL14" s="118" t="n"/>
-      <c r="CM14" s="118" t="n"/>
-      <c r="CN14" s="118" t="n"/>
-      <c r="CO14" s="118" t="n"/>
-      <c r="CP14" s="118" t="n"/>
-      <c r="CQ14" s="126" t="n"/>
     </row>
-    <row customHeight="1" ht="8.25" r="15" s="113">
+    <row customHeight="1" ht="8.25" r="15" s="113" spans="1:95">
       <c r="A15" s="6" t="n"/>
       <c r="B15" s="34" t="n"/>
       <c r="C15" s="7" t="n"/>
@@ -3847,75 +3232,9 @@
       <c r="I15" s="26" t="n"/>
       <c r="J15" s="26" t="n"/>
       <c r="K15" s="26" t="n"/>
-      <c r="L15" s="35" t="inlineStr">
-        <is>
-          <t>(организация, адрес, телефон, факс, банковские реквизиты)</t>
-        </is>
-      </c>
-      <c r="M15" s="122" t="n"/>
-      <c r="N15" s="122" t="n"/>
-      <c r="O15" s="122" t="n"/>
-      <c r="P15" s="122" t="n"/>
-      <c r="Q15" s="122" t="n"/>
-      <c r="R15" s="122" t="n"/>
-      <c r="S15" s="122" t="n"/>
-      <c r="T15" s="122" t="n"/>
-      <c r="U15" s="122" t="n"/>
-      <c r="V15" s="122" t="n"/>
-      <c r="W15" s="122" t="n"/>
-      <c r="X15" s="122" t="n"/>
-      <c r="Y15" s="122" t="n"/>
-      <c r="Z15" s="122" t="n"/>
-      <c r="AA15" s="122" t="n"/>
-      <c r="AB15" s="122" t="n"/>
-      <c r="AC15" s="122" t="n"/>
-      <c r="AD15" s="122" t="n"/>
-      <c r="AE15" s="122" t="n"/>
-      <c r="AF15" s="122" t="n"/>
-      <c r="AG15" s="122" t="n"/>
-      <c r="AH15" s="122" t="n"/>
-      <c r="AI15" s="122" t="n"/>
-      <c r="AJ15" s="122" t="n"/>
-      <c r="AK15" s="122" t="n"/>
-      <c r="AL15" s="122" t="n"/>
-      <c r="AM15" s="122" t="n"/>
-      <c r="AN15" s="122" t="n"/>
-      <c r="AO15" s="122" t="n"/>
-      <c r="AP15" s="122" t="n"/>
-      <c r="AQ15" s="122" t="n"/>
-      <c r="AR15" s="122" t="n"/>
-      <c r="AS15" s="122" t="n"/>
-      <c r="AT15" s="122" t="n"/>
-      <c r="AU15" s="122" t="n"/>
-      <c r="AV15" s="122" t="n"/>
-      <c r="AW15" s="122" t="n"/>
-      <c r="AX15" s="122" t="n"/>
-      <c r="AY15" s="122" t="n"/>
-      <c r="AZ15" s="122" t="n"/>
-      <c r="BA15" s="122" t="n"/>
-      <c r="BB15" s="122" t="n"/>
-      <c r="BC15" s="122" t="n"/>
-      <c r="BD15" s="122" t="n"/>
-      <c r="BE15" s="122" t="n"/>
-      <c r="BF15" s="122" t="n"/>
-      <c r="BG15" s="122" t="n"/>
-      <c r="BH15" s="122" t="n"/>
-      <c r="BI15" s="122" t="n"/>
-      <c r="BJ15" s="122" t="n"/>
-      <c r="BK15" s="122" t="n"/>
-      <c r="BL15" s="122" t="n"/>
-      <c r="BM15" s="122" t="n"/>
-      <c r="BN15" s="122" t="n"/>
-      <c r="BO15" s="122" t="n"/>
-      <c r="BP15" s="122" t="n"/>
-      <c r="BQ15" s="122" t="n"/>
-      <c r="BR15" s="122" t="n"/>
-      <c r="BS15" s="122" t="n"/>
-      <c r="BT15" s="122" t="n"/>
-      <c r="BU15" s="122" t="n"/>
-      <c r="BV15" s="122" t="n"/>
-      <c r="BW15" s="122" t="n"/>
-      <c r="BX15" s="122" t="n"/>
+      <c r="L15" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="BY15" s="34" t="n"/>
       <c r="BZ15" s="34" t="n"/>
       <c r="CA15" s="34" t="n"/>
@@ -3924,24 +3243,11 @@
       <c r="CD15" s="36" t="n"/>
       <c r="CE15" s="17" t="n"/>
       <c r="CF15" s="22" t="n"/>
-      <c r="CG15" s="122" t="n"/>
-      <c r="CH15" s="122" t="n"/>
-      <c r="CI15" s="122" t="n"/>
-      <c r="CJ15" s="122" t="n"/>
-      <c r="CK15" s="122" t="n"/>
-      <c r="CL15" s="122" t="n"/>
-      <c r="CM15" s="122" t="n"/>
-      <c r="CN15" s="122" t="n"/>
-      <c r="CO15" s="122" t="n"/>
-      <c r="CP15" s="122" t="n"/>
-      <c r="CQ15" s="124" t="n"/>
     </row>
-    <row customHeight="1" ht="11.25" r="16" s="113">
+    <row customHeight="1" ht="11.25" r="16" s="113" spans="1:95">
       <c r="A16" s="6" t="n"/>
-      <c r="B16" s="32" t="inlineStr">
-        <is>
-          <t>Плательщик</t>
-        </is>
+      <c r="B16" s="32" t="s">
+        <v>13</v>
       </c>
       <c r="C16" s="7" t="n"/>
       <c r="D16" s="7" t="n"/>
@@ -3950,98 +3256,17 @@
       <c r="G16" s="7" t="n"/>
       <c r="H16" s="7" t="n"/>
       <c r="I16" s="33" t="n"/>
-      <c r="J16" s="118" t="n"/>
-      <c r="K16" s="118" t="n"/>
-      <c r="L16" s="118" t="n"/>
-      <c r="M16" s="118" t="n"/>
-      <c r="N16" s="118" t="n"/>
-      <c r="O16" s="118" t="n"/>
-      <c r="P16" s="118" t="n"/>
-      <c r="Q16" s="118" t="n"/>
-      <c r="R16" s="118" t="n"/>
-      <c r="S16" s="118" t="n"/>
-      <c r="T16" s="118" t="n"/>
-      <c r="U16" s="118" t="n"/>
-      <c r="V16" s="118" t="n"/>
-      <c r="W16" s="118" t="n"/>
-      <c r="X16" s="118" t="n"/>
-      <c r="Y16" s="118" t="n"/>
-      <c r="Z16" s="118" t="n"/>
-      <c r="AA16" s="118" t="n"/>
-      <c r="AB16" s="118" t="n"/>
-      <c r="AC16" s="118" t="n"/>
-      <c r="AD16" s="118" t="n"/>
-      <c r="AE16" s="118" t="n"/>
-      <c r="AF16" s="118" t="n"/>
-      <c r="AG16" s="118" t="n"/>
-      <c r="AH16" s="118" t="n"/>
-      <c r="AI16" s="118" t="n"/>
-      <c r="AJ16" s="118" t="n"/>
-      <c r="AK16" s="118" t="n"/>
-      <c r="AL16" s="118" t="n"/>
-      <c r="AM16" s="118" t="n"/>
-      <c r="AN16" s="118" t="n"/>
-      <c r="AO16" s="118" t="n"/>
-      <c r="AP16" s="118" t="n"/>
-      <c r="AQ16" s="118" t="n"/>
-      <c r="AR16" s="118" t="n"/>
-      <c r="AS16" s="118" t="n"/>
-      <c r="AT16" s="118" t="n"/>
-      <c r="AU16" s="118" t="n"/>
-      <c r="AV16" s="118" t="n"/>
-      <c r="AW16" s="118" t="n"/>
-      <c r="AX16" s="118" t="n"/>
-      <c r="AY16" s="118" t="n"/>
-      <c r="AZ16" s="118" t="n"/>
-      <c r="BA16" s="118" t="n"/>
-      <c r="BB16" s="118" t="n"/>
-      <c r="BC16" s="118" t="n"/>
-      <c r="BD16" s="118" t="n"/>
-      <c r="BE16" s="118" t="n"/>
-      <c r="BF16" s="118" t="n"/>
-      <c r="BG16" s="118" t="n"/>
-      <c r="BH16" s="118" t="n"/>
-      <c r="BI16" s="118" t="n"/>
-      <c r="BJ16" s="118" t="n"/>
-      <c r="BK16" s="118" t="n"/>
-      <c r="BL16" s="118" t="n"/>
-      <c r="BM16" s="118" t="n"/>
-      <c r="BN16" s="118" t="n"/>
-      <c r="BO16" s="118" t="n"/>
-      <c r="BP16" s="118" t="n"/>
-      <c r="BQ16" s="118" t="n"/>
-      <c r="BR16" s="118" t="n"/>
-      <c r="BS16" s="118" t="n"/>
-      <c r="BT16" s="118" t="n"/>
-      <c r="BU16" s="118" t="n"/>
-      <c r="BV16" s="118" t="n"/>
-      <c r="BW16" s="118" t="n"/>
-      <c r="BX16" s="118" t="n"/>
       <c r="BY16" s="37" t="n"/>
       <c r="BZ16" s="37" t="n"/>
       <c r="CA16" s="37" t="n"/>
       <c r="CB16" s="37" t="n"/>
       <c r="CC16" s="37" t="n"/>
-      <c r="CD16" s="38" t="inlineStr">
-        <is>
-          <t>по ОКПО</t>
-        </is>
+      <c r="CD16" s="38" t="s">
+        <v>6</v>
       </c>
       <c r="CE16" s="39" t="n"/>
-      <c r="CF16" s="125" t="n"/>
-      <c r="CG16" s="118" t="n"/>
-      <c r="CH16" s="118" t="n"/>
-      <c r="CI16" s="118" t="n"/>
-      <c r="CJ16" s="118" t="n"/>
-      <c r="CK16" s="118" t="n"/>
-      <c r="CL16" s="118" t="n"/>
-      <c r="CM16" s="118" t="n"/>
-      <c r="CN16" s="118" t="n"/>
-      <c r="CO16" s="118" t="n"/>
-      <c r="CP16" s="118" t="n"/>
-      <c r="CQ16" s="126" t="n"/>
     </row>
-    <row customHeight="1" ht="8.25" r="17" s="113">
+    <row customHeight="1" ht="8.25" r="17" s="113" spans="1:95">
       <c r="A17" s="6" t="n"/>
       <c r="B17" s="34" t="n"/>
       <c r="C17" s="7" t="n"/>
@@ -4053,105 +3278,19 @@
       <c r="I17" s="26" t="n"/>
       <c r="J17" s="26" t="n"/>
       <c r="K17" s="26" t="n"/>
-      <c r="L17" s="40" t="inlineStr">
-        <is>
-          <t>(организация, адрес, телефон, факс, банковские реквизиты)</t>
-        </is>
-      </c>
-      <c r="M17" s="122" t="n"/>
-      <c r="N17" s="122" t="n"/>
-      <c r="O17" s="122" t="n"/>
-      <c r="P17" s="122" t="n"/>
-      <c r="Q17" s="122" t="n"/>
-      <c r="R17" s="122" t="n"/>
-      <c r="S17" s="122" t="n"/>
-      <c r="T17" s="122" t="n"/>
-      <c r="U17" s="122" t="n"/>
-      <c r="V17" s="122" t="n"/>
-      <c r="W17" s="122" t="n"/>
-      <c r="X17" s="122" t="n"/>
-      <c r="Y17" s="122" t="n"/>
-      <c r="Z17" s="122" t="n"/>
-      <c r="AA17" s="122" t="n"/>
-      <c r="AB17" s="122" t="n"/>
-      <c r="AC17" s="122" t="n"/>
-      <c r="AD17" s="122" t="n"/>
-      <c r="AE17" s="122" t="n"/>
-      <c r="AF17" s="122" t="n"/>
-      <c r="AG17" s="122" t="n"/>
-      <c r="AH17" s="122" t="n"/>
-      <c r="AI17" s="122" t="n"/>
-      <c r="AJ17" s="122" t="n"/>
-      <c r="AK17" s="122" t="n"/>
-      <c r="AL17" s="122" t="n"/>
-      <c r="AM17" s="122" t="n"/>
-      <c r="AN17" s="122" t="n"/>
-      <c r="AO17" s="122" t="n"/>
-      <c r="AP17" s="122" t="n"/>
-      <c r="AQ17" s="122" t="n"/>
-      <c r="AR17" s="122" t="n"/>
-      <c r="AS17" s="122" t="n"/>
-      <c r="AT17" s="122" t="n"/>
-      <c r="AU17" s="122" t="n"/>
-      <c r="AV17" s="122" t="n"/>
-      <c r="AW17" s="122" t="n"/>
-      <c r="AX17" s="122" t="n"/>
-      <c r="AY17" s="122" t="n"/>
-      <c r="AZ17" s="122" t="n"/>
-      <c r="BA17" s="122" t="n"/>
-      <c r="BB17" s="122" t="n"/>
-      <c r="BC17" s="122" t="n"/>
-      <c r="BD17" s="122" t="n"/>
-      <c r="BE17" s="122" t="n"/>
-      <c r="BF17" s="122" t="n"/>
-      <c r="BG17" s="122" t="n"/>
-      <c r="BH17" s="122" t="n"/>
-      <c r="BI17" s="122" t="n"/>
-      <c r="BJ17" s="122" t="n"/>
-      <c r="BK17" s="122" t="n"/>
-      <c r="BL17" s="122" t="n"/>
-      <c r="BM17" s="122" t="n"/>
-      <c r="BN17" s="122" t="n"/>
-      <c r="BO17" s="122" t="n"/>
-      <c r="BP17" s="122" t="n"/>
-      <c r="BQ17" s="122" t="n"/>
-      <c r="BR17" s="122" t="n"/>
-      <c r="BS17" s="122" t="n"/>
-      <c r="BT17" s="122" t="n"/>
-      <c r="BU17" s="122" t="n"/>
-      <c r="BV17" s="122" t="n"/>
-      <c r="BW17" s="122" t="n"/>
-      <c r="BX17" s="127" t="n"/>
-      <c r="BY17" s="41" t="inlineStr">
-        <is>
-          <t>номер</t>
-        </is>
-      </c>
-      <c r="BZ17" s="122" t="n"/>
-      <c r="CA17" s="122" t="n"/>
-      <c r="CB17" s="122" t="n"/>
-      <c r="CC17" s="122" t="n"/>
-      <c r="CD17" s="127" t="n"/>
+      <c r="L17" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="BY17" s="41" t="s">
+        <v>14</v>
+      </c>
       <c r="CE17" s="42" t="n"/>
       <c r="CF17" s="22" t="n"/>
-      <c r="CG17" s="122" t="n"/>
-      <c r="CH17" s="122" t="n"/>
-      <c r="CI17" s="122" t="n"/>
-      <c r="CJ17" s="122" t="n"/>
-      <c r="CK17" s="122" t="n"/>
-      <c r="CL17" s="122" t="n"/>
-      <c r="CM17" s="122" t="n"/>
-      <c r="CN17" s="122" t="n"/>
-      <c r="CO17" s="122" t="n"/>
-      <c r="CP17" s="122" t="n"/>
-      <c r="CQ17" s="124" t="n"/>
     </row>
-    <row customHeight="1" ht="10.5" r="18" s="113">
+    <row customHeight="1" ht="10.5" r="18" s="113" spans="1:95">
       <c r="A18" s="6" t="n"/>
-      <c r="B18" s="32" t="inlineStr">
-        <is>
-          <t>Основание</t>
-        </is>
+      <c r="B18" s="32" t="s">
+        <v>15</v>
       </c>
       <c r="C18" s="7" t="n"/>
       <c r="D18" s="7" t="n"/>
@@ -4159,99 +3298,12 @@
       <c r="F18" s="7" t="n"/>
       <c r="G18" s="7" t="n"/>
       <c r="H18" s="7" t="n"/>
-      <c r="I18" s="128" t="inlineStr">
-        <is>
-          <t>swfidhewfihefiherifhweifhiqwehfliqwhe</t>
-        </is>
-      </c>
-      <c r="J18" s="118" t="n"/>
-      <c r="K18" s="118" t="n"/>
-      <c r="L18" s="118" t="n"/>
-      <c r="M18" s="118" t="n"/>
-      <c r="N18" s="118" t="n"/>
-      <c r="O18" s="118" t="n"/>
-      <c r="P18" s="118" t="n"/>
-      <c r="Q18" s="118" t="n"/>
-      <c r="R18" s="118" t="n"/>
-      <c r="S18" s="118" t="n"/>
-      <c r="T18" s="118" t="n"/>
-      <c r="U18" s="118" t="n"/>
-      <c r="V18" s="118" t="n"/>
-      <c r="W18" s="118" t="n"/>
-      <c r="X18" s="118" t="n"/>
-      <c r="Y18" s="118" t="n"/>
-      <c r="Z18" s="118" t="n"/>
-      <c r="AA18" s="118" t="n"/>
-      <c r="AB18" s="118" t="n"/>
-      <c r="AC18" s="118" t="n"/>
-      <c r="AD18" s="118" t="n"/>
-      <c r="AE18" s="118" t="n"/>
-      <c r="AF18" s="118" t="n"/>
-      <c r="AG18" s="118" t="n"/>
-      <c r="AH18" s="118" t="n"/>
-      <c r="AI18" s="118" t="n"/>
-      <c r="AJ18" s="118" t="n"/>
-      <c r="AK18" s="118" t="n"/>
-      <c r="AL18" s="118" t="n"/>
-      <c r="AM18" s="118" t="n"/>
-      <c r="AN18" s="118" t="n"/>
-      <c r="AO18" s="118" t="n"/>
-      <c r="AP18" s="118" t="n"/>
-      <c r="AQ18" s="118" t="n"/>
-      <c r="AR18" s="118" t="n"/>
-      <c r="AS18" s="118" t="n"/>
-      <c r="AT18" s="118" t="n"/>
-      <c r="AU18" s="118" t="n"/>
-      <c r="AV18" s="118" t="n"/>
-      <c r="AW18" s="118" t="n"/>
-      <c r="AX18" s="118" t="n"/>
-      <c r="AY18" s="118" t="n"/>
-      <c r="AZ18" s="118" t="n"/>
-      <c r="BA18" s="118" t="n"/>
-      <c r="BB18" s="118" t="n"/>
-      <c r="BC18" s="118" t="n"/>
-      <c r="BD18" s="118" t="n"/>
-      <c r="BE18" s="118" t="n"/>
-      <c r="BF18" s="118" t="n"/>
-      <c r="BG18" s="118" t="n"/>
-      <c r="BH18" s="118" t="n"/>
-      <c r="BI18" s="118" t="n"/>
-      <c r="BJ18" s="118" t="n"/>
-      <c r="BK18" s="118" t="n"/>
-      <c r="BL18" s="118" t="n"/>
-      <c r="BM18" s="118" t="n"/>
-      <c r="BN18" s="118" t="n"/>
-      <c r="BO18" s="118" t="n"/>
-      <c r="BP18" s="118" t="n"/>
-      <c r="BQ18" s="118" t="n"/>
-      <c r="BR18" s="118" t="n"/>
-      <c r="BS18" s="118" t="n"/>
-      <c r="BT18" s="118" t="n"/>
-      <c r="BU18" s="118" t="n"/>
-      <c r="BV18" s="118" t="n"/>
-      <c r="BW18" s="118" t="n"/>
-      <c r="BX18" s="129" t="n"/>
-      <c r="BY18" s="130" t="n"/>
-      <c r="BZ18" s="118" t="n"/>
-      <c r="CA18" s="118" t="n"/>
-      <c r="CB18" s="118" t="n"/>
-      <c r="CC18" s="118" t="n"/>
-      <c r="CD18" s="129" t="n"/>
+      <c r="I18" s="43" t="s">
+        <v>16</v>
+      </c>
       <c r="CE18" s="45" t="n"/>
-      <c r="CF18" s="125" t="n"/>
-      <c r="CG18" s="118" t="n"/>
-      <c r="CH18" s="118" t="n"/>
-      <c r="CI18" s="118" t="n"/>
-      <c r="CJ18" s="118" t="n"/>
-      <c r="CK18" s="118" t="n"/>
-      <c r="CL18" s="118" t="n"/>
-      <c r="CM18" s="118" t="n"/>
-      <c r="CN18" s="118" t="n"/>
-      <c r="CO18" s="118" t="n"/>
-      <c r="CP18" s="118" t="n"/>
-      <c r="CQ18" s="126" t="n"/>
     </row>
-    <row customHeight="1" ht="8" r="19" s="113">
+    <row customHeight="1" ht="8" r="19" s="113" spans="1:95">
       <c r="A19" s="6" t="n"/>
       <c r="B19" s="7" t="n"/>
       <c r="C19" s="7" t="n"/>
@@ -4263,100 +3315,16 @@
       <c r="I19" s="26" t="n"/>
       <c r="J19" s="26" t="n"/>
       <c r="K19" s="26" t="n"/>
-      <c r="L19" s="40" t="inlineStr">
-        <is>
-          <t>(договор, заказ-наряд)</t>
-        </is>
-      </c>
-      <c r="M19" s="122" t="n"/>
-      <c r="N19" s="122" t="n"/>
-      <c r="O19" s="122" t="n"/>
-      <c r="P19" s="122" t="n"/>
-      <c r="Q19" s="122" t="n"/>
-      <c r="R19" s="122" t="n"/>
-      <c r="S19" s="122" t="n"/>
-      <c r="T19" s="122" t="n"/>
-      <c r="U19" s="122" t="n"/>
-      <c r="V19" s="122" t="n"/>
-      <c r="W19" s="122" t="n"/>
-      <c r="X19" s="122" t="n"/>
-      <c r="Y19" s="122" t="n"/>
-      <c r="Z19" s="122" t="n"/>
-      <c r="AA19" s="122" t="n"/>
-      <c r="AB19" s="122" t="n"/>
-      <c r="AC19" s="122" t="n"/>
-      <c r="AD19" s="122" t="n"/>
-      <c r="AE19" s="122" t="n"/>
-      <c r="AF19" s="122" t="n"/>
-      <c r="AG19" s="122" t="n"/>
-      <c r="AH19" s="122" t="n"/>
-      <c r="AI19" s="122" t="n"/>
-      <c r="AJ19" s="122" t="n"/>
-      <c r="AK19" s="122" t="n"/>
-      <c r="AL19" s="122" t="n"/>
-      <c r="AM19" s="122" t="n"/>
-      <c r="AN19" s="122" t="n"/>
-      <c r="AO19" s="122" t="n"/>
-      <c r="AP19" s="122" t="n"/>
-      <c r="AQ19" s="122" t="n"/>
-      <c r="AR19" s="122" t="n"/>
-      <c r="AS19" s="122" t="n"/>
-      <c r="AT19" s="122" t="n"/>
-      <c r="AU19" s="122" t="n"/>
-      <c r="AV19" s="122" t="n"/>
-      <c r="AW19" s="122" t="n"/>
-      <c r="AX19" s="122" t="n"/>
-      <c r="AY19" s="122" t="n"/>
-      <c r="AZ19" s="122" t="n"/>
-      <c r="BA19" s="122" t="n"/>
-      <c r="BB19" s="122" t="n"/>
-      <c r="BC19" s="122" t="n"/>
-      <c r="BD19" s="122" t="n"/>
-      <c r="BE19" s="122" t="n"/>
-      <c r="BF19" s="122" t="n"/>
-      <c r="BG19" s="122" t="n"/>
-      <c r="BH19" s="122" t="n"/>
-      <c r="BI19" s="122" t="n"/>
-      <c r="BJ19" s="122" t="n"/>
-      <c r="BK19" s="122" t="n"/>
-      <c r="BL19" s="122" t="n"/>
-      <c r="BM19" s="122" t="n"/>
-      <c r="BN19" s="122" t="n"/>
-      <c r="BO19" s="122" t="n"/>
-      <c r="BP19" s="122" t="n"/>
-      <c r="BQ19" s="122" t="n"/>
-      <c r="BR19" s="122" t="n"/>
-      <c r="BS19" s="122" t="n"/>
-      <c r="BT19" s="122" t="n"/>
-      <c r="BU19" s="122" t="n"/>
-      <c r="BV19" s="122" t="n"/>
-      <c r="BW19" s="122" t="n"/>
-      <c r="BX19" s="127" t="n"/>
-      <c r="BY19" s="41" t="inlineStr">
-        <is>
-          <t>дата</t>
-        </is>
-      </c>
-      <c r="BZ19" s="122" t="n"/>
-      <c r="CA19" s="122" t="n"/>
-      <c r="CB19" s="122" t="n"/>
-      <c r="CC19" s="122" t="n"/>
-      <c r="CD19" s="127" t="n"/>
+      <c r="L19" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="BY19" s="41" t="s">
+        <v>18</v>
+      </c>
       <c r="CE19" s="42" t="n"/>
       <c r="CF19" s="22" t="n"/>
-      <c r="CG19" s="122" t="n"/>
-      <c r="CH19" s="122" t="n"/>
-      <c r="CI19" s="122" t="n"/>
-      <c r="CJ19" s="122" t="n"/>
-      <c r="CK19" s="122" t="n"/>
-      <c r="CL19" s="122" t="n"/>
-      <c r="CM19" s="122" t="n"/>
-      <c r="CN19" s="122" t="n"/>
-      <c r="CO19" s="122" t="n"/>
-      <c r="CP19" s="122" t="n"/>
-      <c r="CQ19" s="124" t="n"/>
     </row>
-    <row customHeight="1" ht="10.5" r="20" s="113">
+    <row customHeight="1" ht="10.5" r="20" s="113" spans="1:95">
       <c r="A20" s="6" t="n"/>
       <c r="B20" s="7" t="n"/>
       <c r="C20" s="7" t="n"/>
@@ -4433,27 +3401,9 @@
       <c r="BV20" s="7" t="n"/>
       <c r="BW20" s="7" t="n"/>
       <c r="BX20" s="13" t="n"/>
-      <c r="BY20" s="130" t="n"/>
-      <c r="BZ20" s="118" t="n"/>
-      <c r="CA20" s="118" t="n"/>
-      <c r="CB20" s="118" t="n"/>
-      <c r="CC20" s="118" t="n"/>
-      <c r="CD20" s="129" t="n"/>
       <c r="CE20" s="45" t="n"/>
-      <c r="CF20" s="125" t="n"/>
-      <c r="CG20" s="118" t="n"/>
-      <c r="CH20" s="118" t="n"/>
-      <c r="CI20" s="118" t="n"/>
-      <c r="CJ20" s="118" t="n"/>
-      <c r="CK20" s="118" t="n"/>
-      <c r="CL20" s="118" t="n"/>
-      <c r="CM20" s="118" t="n"/>
-      <c r="CN20" s="118" t="n"/>
-      <c r="CO20" s="118" t="n"/>
-      <c r="CP20" s="118" t="n"/>
-      <c r="CQ20" s="126" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="21" s="113">
+    <row customHeight="1" ht="15.75" r="21" s="113" spans="1:95">
       <c r="A21" s="6" t="n"/>
       <c r="B21" s="7" t="n"/>
       <c r="C21" s="7" t="n"/>
@@ -4517,10 +3467,8 @@
       <c r="BI21" s="7" t="n"/>
       <c r="BJ21" s="7" t="n"/>
       <c r="BK21" s="7" t="n"/>
-      <c r="BL21" s="47" t="inlineStr">
-        <is>
-          <t>Транспортная накладная</t>
-        </is>
+      <c r="BL21" s="47" t="s">
+        <v>19</v>
       </c>
       <c r="BM21" s="7" t="n"/>
       <c r="BN21" s="7" t="n"/>
@@ -4534,31 +3482,13 @@
       <c r="BV21" s="7" t="n"/>
       <c r="BW21" s="7" t="n"/>
       <c r="BX21" s="13" t="n"/>
-      <c r="BY21" s="41" t="inlineStr">
-        <is>
-          <t>номер</t>
-        </is>
-      </c>
-      <c r="BZ21" s="120" t="n"/>
-      <c r="CA21" s="120" t="n"/>
-      <c r="CB21" s="120" t="n"/>
-      <c r="CC21" s="120" t="n"/>
-      <c r="CD21" s="131" t="n"/>
+      <c r="BY21" s="41" t="s">
+        <v>14</v>
+      </c>
       <c r="CE21" s="48" t="n"/>
       <c r="CF21" s="22" t="n"/>
-      <c r="CG21" s="120" t="n"/>
-      <c r="CH21" s="120" t="n"/>
-      <c r="CI21" s="120" t="n"/>
-      <c r="CJ21" s="120" t="n"/>
-      <c r="CK21" s="120" t="n"/>
-      <c r="CL21" s="120" t="n"/>
-      <c r="CM21" s="120" t="n"/>
-      <c r="CN21" s="120" t="n"/>
-      <c r="CO21" s="120" t="n"/>
-      <c r="CP21" s="120" t="n"/>
-      <c r="CQ21" s="121" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="22" s="113">
+    <row customHeight="1" ht="15.75" r="22" s="113" spans="1:95">
       <c r="A22" s="6" t="n"/>
       <c r="B22" s="7" t="n"/>
       <c r="C22" s="7" t="n"/>
@@ -4635,31 +3565,13 @@
       <c r="BV22" s="7" t="n"/>
       <c r="BW22" s="7" t="n"/>
       <c r="BX22" s="13" t="n"/>
-      <c r="BY22" s="41" t="inlineStr">
-        <is>
-          <t>дата</t>
-        </is>
-      </c>
-      <c r="BZ22" s="120" t="n"/>
-      <c r="CA22" s="120" t="n"/>
-      <c r="CB22" s="120" t="n"/>
-      <c r="CC22" s="120" t="n"/>
-      <c r="CD22" s="131" t="n"/>
+      <c r="BY22" s="41" t="s">
+        <v>18</v>
+      </c>
       <c r="CE22" s="48" t="n"/>
       <c r="CF22" s="22" t="n"/>
-      <c r="CG22" s="120" t="n"/>
-      <c r="CH22" s="120" t="n"/>
-      <c r="CI22" s="120" t="n"/>
-      <c r="CJ22" s="120" t="n"/>
-      <c r="CK22" s="120" t="n"/>
-      <c r="CL22" s="120" t="n"/>
-      <c r="CM22" s="120" t="n"/>
-      <c r="CN22" s="120" t="n"/>
-      <c r="CO22" s="120" t="n"/>
-      <c r="CP22" s="120" t="n"/>
-      <c r="CQ22" s="121" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="23" s="113">
+    <row customHeight="1" ht="15.75" r="23" s="113" spans="1:95">
       <c r="A23" s="6" t="n"/>
       <c r="B23" s="7" t="n"/>
       <c r="C23" s="7" t="n"/>
@@ -4741,26 +3653,13 @@
       <c r="CA23" s="49" t="n"/>
       <c r="CB23" s="49" t="n"/>
       <c r="CC23" s="49" t="n"/>
-      <c r="CD23" s="31" t="inlineStr">
-        <is>
-          <t>Вид операции</t>
-        </is>
+      <c r="CD23" s="31" t="s">
+        <v>20</v>
       </c>
       <c r="CE23" s="30" t="n"/>
       <c r="CF23" s="50" t="n"/>
-      <c r="CG23" s="114" t="n"/>
-      <c r="CH23" s="114" t="n"/>
-      <c r="CI23" s="114" t="n"/>
-      <c r="CJ23" s="114" t="n"/>
-      <c r="CK23" s="114" t="n"/>
-      <c r="CL23" s="114" t="n"/>
-      <c r="CM23" s="114" t="n"/>
-      <c r="CN23" s="114" t="n"/>
-      <c r="CO23" s="114" t="n"/>
-      <c r="CP23" s="114" t="n"/>
-      <c r="CQ23" s="132" t="n"/>
     </row>
-    <row customHeight="1" ht="15.5" r="24" s="113">
+    <row customHeight="1" ht="15.5" r="24" s="113" spans="1:95">
       <c r="A24" s="6" t="n"/>
       <c r="B24" s="7" t="n"/>
       <c r="C24" s="7" t="n"/>
@@ -4857,7 +3756,7 @@
       <c r="CP24" s="52" t="n"/>
       <c r="CQ24" s="53" t="n"/>
     </row>
-    <row customHeight="1" ht="26.25" r="25" s="113">
+    <row customHeight="1" ht="26.25" r="25" s="113" spans="1:95">
       <c r="A25" s="6" t="n"/>
       <c r="B25" s="7" t="n"/>
       <c r="C25" s="7" t="n"/>
@@ -4907,38 +3806,12 @@
       <c r="AU25" s="7" t="n"/>
       <c r="AV25" s="7" t="n"/>
       <c r="AW25" s="13" t="n"/>
-      <c r="AX25" s="54" t="inlineStr">
-        <is>
-          <t>Номер
-документа</t>
-        </is>
-      </c>
-      <c r="AY25" s="114" t="n"/>
-      <c r="AZ25" s="114" t="n"/>
-      <c r="BA25" s="114" t="n"/>
-      <c r="BB25" s="114" t="n"/>
-      <c r="BC25" s="114" t="n"/>
-      <c r="BD25" s="114" t="n"/>
-      <c r="BE25" s="114" t="n"/>
-      <c r="BF25" s="114" t="n"/>
-      <c r="BG25" s="114" t="n"/>
-      <c r="BH25" s="115" t="n"/>
-      <c r="BI25" s="54" t="inlineStr">
-        <is>
-          <t>Дата
-составления</t>
-        </is>
-      </c>
-      <c r="BJ25" s="114" t="n"/>
-      <c r="BK25" s="114" t="n"/>
-      <c r="BL25" s="114" t="n"/>
-      <c r="BM25" s="114" t="n"/>
-      <c r="BN25" s="114" t="n"/>
-      <c r="BO25" s="114" t="n"/>
-      <c r="BP25" s="114" t="n"/>
-      <c r="BQ25" s="114" t="n"/>
-      <c r="BR25" s="114" t="n"/>
-      <c r="BS25" s="115" t="n"/>
+      <c r="AX25" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="BI25" s="54" t="s">
+        <v>22</v>
+      </c>
       <c r="BT25" s="55" t="n"/>
       <c r="BU25" s="7" t="n"/>
       <c r="BV25" s="7" t="n"/>
@@ -4964,7 +3837,7 @@
       <c r="CP25" s="7" t="n"/>
       <c r="CQ25" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="18.45" r="26" s="113">
+    <row customHeight="1" ht="18.45" r="26" s="113" spans="1:95">
       <c r="A26" s="6" t="n"/>
       <c r="B26" s="7" t="n"/>
       <c r="C26" s="7" t="n"/>
@@ -4994,10 +3867,8 @@
       <c r="AA26" s="7" t="n"/>
       <c r="AB26" s="7" t="n"/>
       <c r="AC26" s="7" t="n"/>
-      <c r="AD26" s="56" t="inlineStr">
-        <is>
-          <t>ТОВАРНАЯ НАКЛАДНАЯ</t>
-        </is>
+      <c r="AD26" s="56" t="s">
+        <v>23</v>
       </c>
       <c r="AE26" s="7" t="n"/>
       <c r="AF26" s="7" t="n"/>
@@ -5019,27 +3890,7 @@
       <c r="AV26" s="7" t="n"/>
       <c r="AW26" s="17" t="n"/>
       <c r="AX26" s="57" t="n"/>
-      <c r="AY26" s="133" t="n"/>
-      <c r="AZ26" s="133" t="n"/>
-      <c r="BA26" s="133" t="n"/>
-      <c r="BB26" s="133" t="n"/>
-      <c r="BC26" s="133" t="n"/>
-      <c r="BD26" s="133" t="n"/>
-      <c r="BE26" s="133" t="n"/>
-      <c r="BF26" s="133" t="n"/>
-      <c r="BG26" s="133" t="n"/>
-      <c r="BH26" s="134" t="n"/>
       <c r="BI26" s="59" t="n"/>
-      <c r="BJ26" s="133" t="n"/>
-      <c r="BK26" s="133" t="n"/>
-      <c r="BL26" s="133" t="n"/>
-      <c r="BM26" s="133" t="n"/>
-      <c r="BN26" s="133" t="n"/>
-      <c r="BO26" s="133" t="n"/>
-      <c r="BP26" s="133" t="n"/>
-      <c r="BQ26" s="133" t="n"/>
-      <c r="BR26" s="133" t="n"/>
-      <c r="BS26" s="135" t="n"/>
       <c r="BT26" s="61" t="n"/>
       <c r="BU26" s="7" t="n"/>
       <c r="BV26" s="7" t="n"/>
@@ -5065,7 +3916,7 @@
       <c r="CP26" s="7" t="n"/>
       <c r="CQ26" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="27" s="113">
+    <row customHeight="1" ht="12" r="27" s="113" spans="1:95">
       <c r="A27" s="62" t="n"/>
       <c r="B27" s="11" t="n"/>
       <c r="C27" s="11" t="n"/>
@@ -5162,438 +4013,121 @@
       <c r="CP27" s="11" t="n"/>
       <c r="CQ27" s="12" t="n"/>
     </row>
-    <row customHeight="1" ht="26.25" r="28" s="113">
-      <c r="A28" s="64" t="inlineStr">
-        <is>
-          <t>Но- мер по по- рядку</t>
-        </is>
-      </c>
-      <c r="B28" s="122" t="n"/>
-      <c r="C28" s="127" t="n"/>
-      <c r="D28" s="65" t="inlineStr">
-        <is>
-          <t>Товар</t>
-        </is>
-      </c>
-      <c r="E28" s="120" t="n"/>
-      <c r="F28" s="120" t="n"/>
-      <c r="G28" s="120" t="n"/>
-      <c r="H28" s="120" t="n"/>
-      <c r="I28" s="120" t="n"/>
-      <c r="J28" s="120" t="n"/>
-      <c r="K28" s="120" t="n"/>
-      <c r="L28" s="120" t="n"/>
-      <c r="M28" s="120" t="n"/>
-      <c r="N28" s="120" t="n"/>
-      <c r="O28" s="120" t="n"/>
-      <c r="P28" s="120" t="n"/>
-      <c r="Q28" s="120" t="n"/>
-      <c r="R28" s="120" t="n"/>
-      <c r="S28" s="120" t="n"/>
-      <c r="T28" s="120" t="n"/>
-      <c r="U28" s="120" t="n"/>
-      <c r="V28" s="120" t="n"/>
-      <c r="W28" s="131" t="n"/>
-      <c r="X28" s="66" t="inlineStr">
-        <is>
-          <t>Единица
-измерения</t>
-        </is>
-      </c>
-      <c r="Y28" s="120" t="n"/>
-      <c r="Z28" s="120" t="n"/>
-      <c r="AA28" s="120" t="n"/>
-      <c r="AB28" s="120" t="n"/>
-      <c r="AC28" s="120" t="n"/>
-      <c r="AD28" s="120" t="n"/>
-      <c r="AE28" s="120" t="n"/>
-      <c r="AF28" s="120" t="n"/>
-      <c r="AG28" s="131" t="n"/>
-      <c r="AH28" s="66" t="inlineStr">
-        <is>
-          <t>Вид упаков- ки</t>
-        </is>
-      </c>
-      <c r="AI28" s="122" t="n"/>
-      <c r="AJ28" s="122" t="n"/>
-      <c r="AK28" s="122" t="n"/>
-      <c r="AL28" s="127" t="n"/>
-      <c r="AM28" s="66" t="inlineStr">
-        <is>
-          <t>Количество</t>
-        </is>
-      </c>
-      <c r="AN28" s="120" t="n"/>
-      <c r="AO28" s="120" t="n"/>
-      <c r="AP28" s="120" t="n"/>
-      <c r="AQ28" s="120" t="n"/>
-      <c r="AR28" s="120" t="n"/>
-      <c r="AS28" s="120" t="n"/>
-      <c r="AT28" s="120" t="n"/>
-      <c r="AU28" s="120" t="n"/>
-      <c r="AV28" s="131" t="n"/>
-      <c r="AW28" s="66" t="inlineStr">
-        <is>
-          <t>Масса брутто</t>
-        </is>
-      </c>
-      <c r="AX28" s="122" t="n"/>
-      <c r="AY28" s="122" t="n"/>
-      <c r="AZ28" s="122" t="n"/>
-      <c r="BA28" s="127" t="n"/>
-      <c r="BB28" s="66" t="inlineStr">
-        <is>
-          <t>Количест- во
-(масса нетто)</t>
-        </is>
-      </c>
-      <c r="BC28" s="122" t="n"/>
-      <c r="BD28" s="122" t="n"/>
-      <c r="BE28" s="122" t="n"/>
-      <c r="BF28" s="122" t="n"/>
-      <c r="BG28" s="127" t="n"/>
-      <c r="BH28" s="66" t="inlineStr">
-        <is>
-          <t>Цена,
-руб. коп.</t>
-        </is>
-      </c>
-      <c r="BI28" s="122" t="n"/>
-      <c r="BJ28" s="122" t="n"/>
-      <c r="BK28" s="122" t="n"/>
-      <c r="BL28" s="122" t="n"/>
-      <c r="BM28" s="122" t="n"/>
-      <c r="BN28" s="122" t="n"/>
-      <c r="BO28" s="122" t="n"/>
-      <c r="BP28" s="127" t="n"/>
-      <c r="BQ28" s="66" t="inlineStr">
-        <is>
-          <t>Сумма без учета НДС, руб. коп.</t>
-        </is>
-      </c>
-      <c r="BR28" s="122" t="n"/>
-      <c r="BS28" s="122" t="n"/>
-      <c r="BT28" s="122" t="n"/>
-      <c r="BU28" s="122" t="n"/>
-      <c r="BV28" s="122" t="n"/>
-      <c r="BW28" s="127" t="n"/>
-      <c r="BX28" s="66" t="inlineStr">
-        <is>
-          <t>НДС</t>
-        </is>
-      </c>
-      <c r="BY28" s="120" t="n"/>
-      <c r="BZ28" s="120" t="n"/>
-      <c r="CA28" s="120" t="n"/>
-      <c r="CB28" s="120" t="n"/>
-      <c r="CC28" s="120" t="n"/>
-      <c r="CD28" s="120" t="n"/>
-      <c r="CE28" s="120" t="n"/>
-      <c r="CF28" s="120" t="n"/>
-      <c r="CG28" s="120" t="n"/>
-      <c r="CH28" s="131" t="n"/>
-      <c r="CI28" s="66" t="inlineStr">
-        <is>
-          <t>Сумма с учетом НДС,
-руб. коп.</t>
-        </is>
-      </c>
-      <c r="CJ28" s="122" t="n"/>
-      <c r="CK28" s="122" t="n"/>
-      <c r="CL28" s="122" t="n"/>
-      <c r="CM28" s="122" t="n"/>
-      <c r="CN28" s="122" t="n"/>
-      <c r="CO28" s="122" t="n"/>
-      <c r="CP28" s="122" t="n"/>
-      <c r="CQ28" s="127" t="n"/>
+    <row customHeight="1" ht="26.25" r="28" s="113" spans="1:95">
+      <c r="A28" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="X28" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH28" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM28" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW28" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="BB28" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="BH28" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="BQ28" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="BX28" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="CI28" s="66" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row customHeight="1" ht="33.75" r="29" s="113">
-      <c r="A29" s="130" t="n"/>
-      <c r="B29" s="118" t="n"/>
-      <c r="C29" s="129" t="n"/>
-      <c r="D29" s="66" t="inlineStr">
-        <is>
-          <t>наименование,
-характеристика, сорт, артикул
-товара</t>
-        </is>
-      </c>
-      <c r="E29" s="120" t="n"/>
-      <c r="F29" s="120" t="n"/>
-      <c r="G29" s="120" t="n"/>
-      <c r="H29" s="120" t="n"/>
-      <c r="I29" s="120" t="n"/>
-      <c r="J29" s="120" t="n"/>
-      <c r="K29" s="120" t="n"/>
-      <c r="L29" s="120" t="n"/>
-      <c r="M29" s="120" t="n"/>
-      <c r="N29" s="120" t="n"/>
-      <c r="O29" s="120" t="n"/>
-      <c r="P29" s="120" t="n"/>
-      <c r="Q29" s="120" t="n"/>
-      <c r="R29" s="120" t="n"/>
-      <c r="S29" s="131" t="n"/>
-      <c r="T29" s="65" t="inlineStr">
-        <is>
-          <t>код</t>
-        </is>
-      </c>
-      <c r="U29" s="120" t="n"/>
-      <c r="V29" s="120" t="n"/>
-      <c r="W29" s="131" t="n"/>
-      <c r="X29" s="66" t="inlineStr">
-        <is>
-          <t>наиме- нование</t>
-        </is>
-      </c>
-      <c r="Y29" s="120" t="n"/>
-      <c r="Z29" s="120" t="n"/>
-      <c r="AA29" s="120" t="n"/>
-      <c r="AB29" s="131" t="n"/>
-      <c r="AC29" s="66" t="inlineStr">
-        <is>
-          <t>код по ОКЕИ</t>
-        </is>
-      </c>
-      <c r="AD29" s="120" t="n"/>
-      <c r="AE29" s="120" t="n"/>
-      <c r="AF29" s="120" t="n"/>
-      <c r="AG29" s="131" t="n"/>
-      <c r="AH29" s="130" t="n"/>
-      <c r="AI29" s="118" t="n"/>
-      <c r="AJ29" s="118" t="n"/>
-      <c r="AK29" s="118" t="n"/>
-      <c r="AL29" s="129" t="n"/>
-      <c r="AM29" s="66" t="inlineStr">
-        <is>
-          <t>в одном месте</t>
-        </is>
-      </c>
-      <c r="AN29" s="120" t="n"/>
-      <c r="AO29" s="120" t="n"/>
-      <c r="AP29" s="120" t="n"/>
-      <c r="AQ29" s="131" t="n"/>
-      <c r="AR29" s="66" t="inlineStr">
-        <is>
-          <t>мест, штук</t>
-        </is>
-      </c>
-      <c r="AS29" s="120" t="n"/>
-      <c r="AT29" s="120" t="n"/>
-      <c r="AU29" s="120" t="n"/>
-      <c r="AV29" s="131" t="n"/>
-      <c r="AW29" s="130" t="n"/>
-      <c r="AX29" s="118" t="n"/>
-      <c r="AY29" s="118" t="n"/>
-      <c r="AZ29" s="118" t="n"/>
-      <c r="BA29" s="129" t="n"/>
-      <c r="BB29" s="130" t="n"/>
-      <c r="BC29" s="118" t="n"/>
-      <c r="BD29" s="118" t="n"/>
-      <c r="BE29" s="118" t="n"/>
-      <c r="BF29" s="118" t="n"/>
-      <c r="BG29" s="129" t="n"/>
-      <c r="BH29" s="130" t="n"/>
-      <c r="BI29" s="118" t="n"/>
-      <c r="BJ29" s="118" t="n"/>
-      <c r="BK29" s="118" t="n"/>
-      <c r="BL29" s="118" t="n"/>
-      <c r="BM29" s="118" t="n"/>
-      <c r="BN29" s="118" t="n"/>
-      <c r="BO29" s="118" t="n"/>
-      <c r="BP29" s="129" t="n"/>
-      <c r="BQ29" s="130" t="n"/>
-      <c r="BR29" s="118" t="n"/>
-      <c r="BS29" s="118" t="n"/>
-      <c r="BT29" s="118" t="n"/>
-      <c r="BU29" s="118" t="n"/>
-      <c r="BV29" s="118" t="n"/>
-      <c r="BW29" s="129" t="n"/>
-      <c r="BX29" s="67" t="inlineStr">
-        <is>
-          <t>ставка, %</t>
-        </is>
-      </c>
-      <c r="BY29" s="120" t="n"/>
-      <c r="BZ29" s="120" t="n"/>
-      <c r="CA29" s="131" t="n"/>
-      <c r="CB29" s="67" t="inlineStr">
-        <is>
-          <t>сумма,
-руб. коп.</t>
-        </is>
-      </c>
-      <c r="CC29" s="120" t="n"/>
-      <c r="CD29" s="120" t="n"/>
-      <c r="CE29" s="120" t="n"/>
-      <c r="CF29" s="120" t="n"/>
-      <c r="CG29" s="120" t="n"/>
-      <c r="CH29" s="131" t="n"/>
-      <c r="CI29" s="130" t="n"/>
-      <c r="CJ29" s="118" t="n"/>
-      <c r="CK29" s="118" t="n"/>
-      <c r="CL29" s="118" t="n"/>
-      <c r="CM29" s="118" t="n"/>
-      <c r="CN29" s="118" t="n"/>
-      <c r="CO29" s="118" t="n"/>
-      <c r="CP29" s="118" t="n"/>
-      <c r="CQ29" s="129" t="n"/>
+    <row customHeight="1" ht="33.75" r="29" s="113" spans="1:95">
+      <c r="D29" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="T29" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="X29" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC29" s="66" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM29" s="66" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR29" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="BX29" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="CB29" s="67" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row customHeight="1" ht="15.5" r="30" s="113">
+    <row customHeight="1" ht="15.5" r="30" s="113" spans="1:95">
       <c r="A30" s="68" t="n">
         <v>1</v>
       </c>
-      <c r="B30" s="120" t="n"/>
-      <c r="C30" s="131" t="n"/>
       <c r="D30" s="68" t="n">
         <v>2</v>
       </c>
-      <c r="E30" s="120" t="n"/>
-      <c r="F30" s="120" t="n"/>
-      <c r="G30" s="120" t="n"/>
-      <c r="H30" s="120" t="n"/>
-      <c r="I30" s="120" t="n"/>
-      <c r="J30" s="120" t="n"/>
-      <c r="K30" s="120" t="n"/>
-      <c r="L30" s="120" t="n"/>
-      <c r="M30" s="120" t="n"/>
-      <c r="N30" s="120" t="n"/>
-      <c r="O30" s="120" t="n"/>
-      <c r="P30" s="120" t="n"/>
-      <c r="Q30" s="120" t="n"/>
-      <c r="R30" s="120" t="n"/>
-      <c r="S30" s="131" t="n"/>
       <c r="T30" s="69" t="n">
         <v>3</v>
       </c>
-      <c r="U30" s="114" t="n"/>
-      <c r="V30" s="114" t="n"/>
-      <c r="W30" s="115" t="n"/>
       <c r="X30" s="68" t="n">
         <v>4</v>
       </c>
-      <c r="Y30" s="120" t="n"/>
-      <c r="Z30" s="120" t="n"/>
-      <c r="AA30" s="120" t="n"/>
-      <c r="AB30" s="131" t="n"/>
       <c r="AC30" s="69" t="n">
         <v>5</v>
       </c>
-      <c r="AD30" s="114" t="n"/>
-      <c r="AE30" s="114" t="n"/>
-      <c r="AF30" s="114" t="n"/>
-      <c r="AG30" s="115" t="n"/>
       <c r="AH30" s="69" t="n">
         <v>6</v>
       </c>
-      <c r="AI30" s="114" t="n"/>
-      <c r="AJ30" s="114" t="n"/>
-      <c r="AK30" s="114" t="n"/>
-      <c r="AL30" s="115" t="n"/>
       <c r="AM30" s="69" t="n">
         <v>7</v>
       </c>
-      <c r="AN30" s="114" t="n"/>
-      <c r="AO30" s="114" t="n"/>
-      <c r="AP30" s="114" t="n"/>
-      <c r="AQ30" s="115" t="n"/>
       <c r="AR30" s="69" t="n">
         <v>8</v>
       </c>
-      <c r="AS30" s="114" t="n"/>
-      <c r="AT30" s="114" t="n"/>
-      <c r="AU30" s="114" t="n"/>
-      <c r="AV30" s="115" t="n"/>
       <c r="AW30" s="69" t="n">
         <v>9</v>
       </c>
-      <c r="AX30" s="114" t="n"/>
-      <c r="AY30" s="114" t="n"/>
-      <c r="AZ30" s="114" t="n"/>
-      <c r="BA30" s="115" t="n"/>
       <c r="BB30" s="69" t="n">
         <v>10</v>
       </c>
-      <c r="BC30" s="114" t="n"/>
-      <c r="BD30" s="114" t="n"/>
-      <c r="BE30" s="114" t="n"/>
-      <c r="BF30" s="114" t="n"/>
-      <c r="BG30" s="115" t="n"/>
       <c r="BH30" s="69" t="n">
         <v>11</v>
       </c>
-      <c r="BI30" s="114" t="n"/>
-      <c r="BJ30" s="114" t="n"/>
-      <c r="BK30" s="114" t="n"/>
-      <c r="BL30" s="114" t="n"/>
-      <c r="BM30" s="114" t="n"/>
-      <c r="BN30" s="114" t="n"/>
-      <c r="BO30" s="114" t="n"/>
-      <c r="BP30" s="115" t="n"/>
       <c r="BQ30" s="69" t="n">
         <v>12</v>
       </c>
-      <c r="BR30" s="114" t="n"/>
-      <c r="BS30" s="114" t="n"/>
-      <c r="BT30" s="114" t="n"/>
-      <c r="BU30" s="114" t="n"/>
-      <c r="BV30" s="114" t="n"/>
-      <c r="BW30" s="115" t="n"/>
       <c r="BX30" s="68" t="n">
         <v>13</v>
       </c>
-      <c r="BY30" s="120" t="n"/>
-      <c r="BZ30" s="120" t="n"/>
-      <c r="CA30" s="131" t="n"/>
       <c r="CB30" s="69" t="n">
         <v>14</v>
       </c>
-      <c r="CC30" s="114" t="n"/>
-      <c r="CD30" s="114" t="n"/>
-      <c r="CE30" s="114" t="n"/>
-      <c r="CF30" s="114" t="n"/>
-      <c r="CG30" s="114" t="n"/>
-      <c r="CH30" s="115" t="n"/>
       <c r="CI30" s="69" t="n">
         <v>15</v>
       </c>
-      <c r="CJ30" s="114" t="n"/>
-      <c r="CK30" s="114" t="n"/>
-      <c r="CL30" s="114" t="n"/>
-      <c r="CM30" s="114" t="n"/>
-      <c r="CN30" s="114" t="n"/>
-      <c r="CO30" s="114" t="n"/>
-      <c r="CP30" s="114" t="n"/>
-      <c r="CQ30" s="115" t="n"/>
     </row>
-    <row customHeight="1" ht="15.5" r="31" s="113">
-      <c r="A31" s="70" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="B31" s="122" t="n"/>
-      <c r="C31" s="122" t="n"/>
-      <c r="D31" s="26" t="inlineStr">
-        <is>
-          <t>testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest</t>
-        </is>
-      </c>
-      <c r="E31" s="122" t="n"/>
-      <c r="F31" s="122" t="n"/>
-      <c r="G31" s="122" t="n"/>
-      <c r="H31" s="122" t="n"/>
-      <c r="I31" s="122" t="n"/>
-      <c r="J31" s="122" t="n"/>
-      <c r="K31" s="122" t="n"/>
-      <c r="L31" s="122" t="n"/>
-      <c r="M31" s="122" t="n"/>
-      <c r="N31" s="122" t="n"/>
-      <c r="O31" s="122" t="n"/>
-      <c r="P31" s="122" t="n"/>
-      <c r="Q31" s="122" t="n"/>
-      <c r="R31" s="122" t="n"/>
-      <c r="S31" s="122" t="n"/>
+    <row customHeight="1" ht="15.5" r="31" s="113" spans="1:95">
+      <c r="A31" s="114" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="114" t="s">
+        <v>44</v>
+      </c>
       <c r="T31" s="52" t="n"/>
       <c r="U31" s="52" t="n"/>
       <c r="V31" s="52" t="n"/>
@@ -5671,81 +4205,21 @@
       <c r="CP31" s="52" t="n"/>
       <c r="CQ31" s="53" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="32" s="113">
-      <c r="A32" s="6" t="n"/>
-      <c r="B32" s="7" t="n"/>
-      <c r="C32" s="7" t="n"/>
-      <c r="D32" s="72" t="inlineStr">
-        <is>
-          <t>Товарная накладная имеет приложение на</t>
-        </is>
-      </c>
-      <c r="E32" s="7" t="n"/>
-      <c r="F32" s="7" t="n"/>
-      <c r="G32" s="7" t="n"/>
-      <c r="H32" s="7" t="n"/>
-      <c r="I32" s="7" t="n"/>
-      <c r="J32" s="7" t="n"/>
-      <c r="K32" s="7" t="n"/>
-      <c r="L32" s="7" t="n"/>
-      <c r="M32" s="7" t="n"/>
-      <c r="N32" s="7" t="n"/>
-      <c r="O32" s="7" t="n"/>
-      <c r="P32" s="7" t="n"/>
-      <c r="Q32" s="7" t="n"/>
-      <c r="R32" s="7" t="n"/>
-      <c r="S32" s="7" t="n"/>
+    <row customHeight="1" ht="15" r="32" s="113" spans="1:95">
+      <c r="A32" s="114" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="115" t="s">
+        <v>46</v>
+      </c>
       <c r="T32" s="7" t="n"/>
       <c r="U32" s="7" t="n"/>
       <c r="V32" s="7" t="n"/>
       <c r="W32" s="7" t="n"/>
       <c r="X32" s="7" t="n"/>
       <c r="Y32" s="11" t="n"/>
-      <c r="Z32" s="118" t="n"/>
-      <c r="AA32" s="118" t="n"/>
-      <c r="AB32" s="118" t="n"/>
-      <c r="AC32" s="118" t="n"/>
-      <c r="AD32" s="118" t="n"/>
-      <c r="AE32" s="118" t="n"/>
-      <c r="AF32" s="118" t="n"/>
-      <c r="AG32" s="118" t="n"/>
-      <c r="AH32" s="118" t="n"/>
-      <c r="AI32" s="118" t="n"/>
-      <c r="AJ32" s="118" t="n"/>
-      <c r="AK32" s="118" t="n"/>
-      <c r="AL32" s="118" t="n"/>
-      <c r="AM32" s="118" t="n"/>
-      <c r="AN32" s="118" t="n"/>
-      <c r="AO32" s="118" t="n"/>
-      <c r="AP32" s="118" t="n"/>
-      <c r="AQ32" s="118" t="n"/>
-      <c r="AR32" s="118" t="n"/>
-      <c r="AS32" s="118" t="n"/>
-      <c r="AT32" s="118" t="n"/>
-      <c r="AU32" s="118" t="n"/>
-      <c r="AV32" s="118" t="n"/>
-      <c r="AW32" s="118" t="n"/>
-      <c r="AX32" s="118" t="n"/>
-      <c r="AY32" s="118" t="n"/>
-      <c r="AZ32" s="118" t="n"/>
-      <c r="BA32" s="118" t="n"/>
-      <c r="BB32" s="118" t="n"/>
-      <c r="BC32" s="118" t="n"/>
-      <c r="BD32" s="118" t="n"/>
-      <c r="BE32" s="118" t="n"/>
-      <c r="BF32" s="118" t="n"/>
-      <c r="BG32" s="118" t="n"/>
-      <c r="BH32" s="118" t="n"/>
-      <c r="BI32" s="118" t="n"/>
-      <c r="BJ32" s="118" t="n"/>
-      <c r="BK32" s="118" t="n"/>
-      <c r="BL32" s="118" t="n"/>
-      <c r="BM32" s="118" t="n"/>
-      <c r="BN32" s="118" t="n"/>
-      <c r="BO32" s="72" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   листах</t>
-        </is>
+      <c r="BO32" s="72" t="s">
+        <v>47</v>
       </c>
       <c r="BP32" s="7" t="n"/>
       <c r="BQ32" s="7" t="n"/>
@@ -5776,14 +4250,12 @@
       <c r="CP32" s="7" t="n"/>
       <c r="CQ32" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="33" s="113">
+    <row customHeight="1" ht="15" r="33" s="113" spans="1:95">
       <c r="A33" s="6" t="n"/>
       <c r="B33" s="7" t="n"/>
       <c r="C33" s="7" t="n"/>
-      <c r="D33" s="72" t="inlineStr">
-        <is>
-          <t>и содержит</t>
-        </is>
+      <c r="D33" s="72" t="s">
+        <v>48</v>
       </c>
       <c r="E33" s="7" t="n"/>
       <c r="F33" s="7" t="n"/>
@@ -5792,65 +4264,8 @@
       <c r="I33" s="7" t="n"/>
       <c r="J33" s="7" t="n"/>
       <c r="K33" s="73" t="n"/>
-      <c r="L33" s="118" t="n"/>
-      <c r="M33" s="118" t="n"/>
-      <c r="N33" s="118" t="n"/>
-      <c r="O33" s="118" t="n"/>
-      <c r="P33" s="118" t="n"/>
-      <c r="Q33" s="118" t="n"/>
-      <c r="R33" s="118" t="n"/>
-      <c r="S33" s="118" t="n"/>
-      <c r="T33" s="118" t="n"/>
-      <c r="U33" s="118" t="n"/>
-      <c r="V33" s="118" t="n"/>
-      <c r="W33" s="118" t="n"/>
-      <c r="X33" s="118" t="n"/>
-      <c r="Y33" s="118" t="n"/>
-      <c r="Z33" s="118" t="n"/>
-      <c r="AA33" s="118" t="n"/>
-      <c r="AB33" s="118" t="n"/>
-      <c r="AC33" s="118" t="n"/>
-      <c r="AD33" s="118" t="n"/>
-      <c r="AE33" s="118" t="n"/>
-      <c r="AF33" s="118" t="n"/>
-      <c r="AG33" s="118" t="n"/>
-      <c r="AH33" s="118" t="n"/>
-      <c r="AI33" s="118" t="n"/>
-      <c r="AJ33" s="118" t="n"/>
-      <c r="AK33" s="118" t="n"/>
-      <c r="AL33" s="118" t="n"/>
-      <c r="AM33" s="118" t="n"/>
-      <c r="AN33" s="118" t="n"/>
-      <c r="AO33" s="118" t="n"/>
-      <c r="AP33" s="118" t="n"/>
-      <c r="AQ33" s="118" t="n"/>
-      <c r="AR33" s="118" t="n"/>
-      <c r="AS33" s="118" t="n"/>
-      <c r="AT33" s="118" t="n"/>
-      <c r="AU33" s="118" t="n"/>
-      <c r="AV33" s="118" t="n"/>
-      <c r="AW33" s="118" t="n"/>
-      <c r="AX33" s="118" t="n"/>
-      <c r="AY33" s="118" t="n"/>
-      <c r="AZ33" s="118" t="n"/>
-      <c r="BA33" s="118" t="n"/>
-      <c r="BB33" s="118" t="n"/>
-      <c r="BC33" s="118" t="n"/>
-      <c r="BD33" s="118" t="n"/>
-      <c r="BE33" s="118" t="n"/>
-      <c r="BF33" s="118" t="n"/>
-      <c r="BG33" s="118" t="n"/>
-      <c r="BH33" s="118" t="n"/>
-      <c r="BI33" s="118" t="n"/>
-      <c r="BJ33" s="118" t="n"/>
-      <c r="BK33" s="118" t="n"/>
-      <c r="BL33" s="118" t="n"/>
-      <c r="BM33" s="118" t="n"/>
-      <c r="BN33" s="118" t="n"/>
-      <c r="BO33" s="72" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   порядковых номеров записей</t>
-        </is>
+      <c r="BO33" s="72" t="s">
+        <v>49</v>
       </c>
       <c r="BP33" s="7" t="n"/>
       <c r="BQ33" s="7" t="n"/>
@@ -5881,7 +4296,7 @@
       <c r="CP33" s="7" t="n"/>
       <c r="CQ33" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="8" r="34" s="113">
+    <row customHeight="1" ht="8" r="34" s="113" spans="1:95">
       <c r="A34" s="6" t="n"/>
       <c r="B34" s="7" t="n"/>
       <c r="C34" s="7" t="n"/>
@@ -5892,66 +4307,9 @@
       <c r="H34" s="7" t="n"/>
       <c r="I34" s="7" t="n"/>
       <c r="J34" s="7" t="n"/>
-      <c r="K34" s="35" t="inlineStr">
-        <is>
-          <t>(прописью)</t>
-        </is>
-      </c>
-      <c r="L34" s="122" t="n"/>
-      <c r="M34" s="122" t="n"/>
-      <c r="N34" s="122" t="n"/>
-      <c r="O34" s="122" t="n"/>
-      <c r="P34" s="122" t="n"/>
-      <c r="Q34" s="122" t="n"/>
-      <c r="R34" s="122" t="n"/>
-      <c r="S34" s="122" t="n"/>
-      <c r="T34" s="122" t="n"/>
-      <c r="U34" s="122" t="n"/>
-      <c r="V34" s="122" t="n"/>
-      <c r="W34" s="122" t="n"/>
-      <c r="X34" s="122" t="n"/>
-      <c r="Y34" s="122" t="n"/>
-      <c r="Z34" s="122" t="n"/>
-      <c r="AA34" s="122" t="n"/>
-      <c r="AB34" s="122" t="n"/>
-      <c r="AC34" s="122" t="n"/>
-      <c r="AD34" s="122" t="n"/>
-      <c r="AE34" s="122" t="n"/>
-      <c r="AF34" s="122" t="n"/>
-      <c r="AG34" s="122" t="n"/>
-      <c r="AH34" s="122" t="n"/>
-      <c r="AI34" s="122" t="n"/>
-      <c r="AJ34" s="122" t="n"/>
-      <c r="AK34" s="122" t="n"/>
-      <c r="AL34" s="122" t="n"/>
-      <c r="AM34" s="122" t="n"/>
-      <c r="AN34" s="122" t="n"/>
-      <c r="AO34" s="122" t="n"/>
-      <c r="AP34" s="122" t="n"/>
-      <c r="AQ34" s="122" t="n"/>
-      <c r="AR34" s="122" t="n"/>
-      <c r="AS34" s="122" t="n"/>
-      <c r="AT34" s="122" t="n"/>
-      <c r="AU34" s="122" t="n"/>
-      <c r="AV34" s="122" t="n"/>
-      <c r="AW34" s="122" t="n"/>
-      <c r="AX34" s="122" t="n"/>
-      <c r="AY34" s="122" t="n"/>
-      <c r="AZ34" s="122" t="n"/>
-      <c r="BA34" s="122" t="n"/>
-      <c r="BB34" s="122" t="n"/>
-      <c r="BC34" s="122" t="n"/>
-      <c r="BD34" s="122" t="n"/>
-      <c r="BE34" s="122" t="n"/>
-      <c r="BF34" s="122" t="n"/>
-      <c r="BG34" s="122" t="n"/>
-      <c r="BH34" s="122" t="n"/>
-      <c r="BI34" s="122" t="n"/>
-      <c r="BJ34" s="122" t="n"/>
-      <c r="BK34" s="122" t="n"/>
-      <c r="BL34" s="122" t="n"/>
-      <c r="BM34" s="122" t="n"/>
-      <c r="BN34" s="122" t="n"/>
+      <c r="K34" s="35" t="s">
+        <v>50</v>
+      </c>
       <c r="BO34" s="7" t="n"/>
       <c r="BP34" s="7" t="n"/>
       <c r="BQ34" s="7" t="n"/>
@@ -5982,7 +4340,7 @@
       <c r="CP34" s="7" t="n"/>
       <c r="CQ34" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="8" r="35" s="113">
+    <row customHeight="1" ht="8" r="35" s="113" spans="1:95">
       <c r="A35" s="6" t="n"/>
       <c r="B35" s="7" t="n"/>
       <c r="C35" s="7" t="n"/>
@@ -6079,7 +4437,7 @@
       <c r="CP35" s="76" t="n"/>
       <c r="CQ35" s="77" t="n"/>
     </row>
-    <row customHeight="1" ht="8" r="36" s="113">
+    <row customHeight="1" ht="8" r="36" s="113" spans="1:95">
       <c r="A36" s="6" t="n"/>
       <c r="B36" s="7" t="n"/>
       <c r="C36" s="7" t="n"/>
@@ -6159,24 +4517,8 @@
       <c r="BY36" s="7" t="n"/>
       <c r="BZ36" s="17" t="n"/>
       <c r="CA36" s="78" t="n"/>
-      <c r="CB36" s="136" t="n"/>
-      <c r="CC36" s="136" t="n"/>
-      <c r="CD36" s="136" t="n"/>
-      <c r="CE36" s="136" t="n"/>
-      <c r="CF36" s="136" t="n"/>
-      <c r="CG36" s="136" t="n"/>
-      <c r="CH36" s="136" t="n"/>
-      <c r="CI36" s="136" t="n"/>
-      <c r="CJ36" s="136" t="n"/>
-      <c r="CK36" s="136" t="n"/>
-      <c r="CL36" s="136" t="n"/>
-      <c r="CM36" s="136" t="n"/>
-      <c r="CN36" s="136" t="n"/>
-      <c r="CO36" s="136" t="n"/>
-      <c r="CP36" s="136" t="n"/>
-      <c r="CQ36" s="137" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="37" s="113">
+    <row customHeight="1" ht="15" r="37" s="113" spans="1:95">
       <c r="A37" s="6" t="n"/>
       <c r="B37" s="7" t="n"/>
       <c r="C37" s="7" t="n"/>
@@ -6205,10 +4547,8 @@
       <c r="Z37" s="7" t="n"/>
       <c r="AA37" s="7" t="n"/>
       <c r="AB37" s="7" t="n"/>
-      <c r="AC37" s="72" t="inlineStr">
-        <is>
-          <t>Масса груза (нетто)</t>
-        </is>
+      <c r="AC37" s="72" t="s">
+        <v>51</v>
       </c>
       <c r="AD37" s="7" t="n"/>
       <c r="AE37" s="7" t="n"/>
@@ -6221,63 +4561,9 @@
       <c r="AL37" s="7" t="n"/>
       <c r="AM37" s="7" t="n"/>
       <c r="AN37" s="11" t="n"/>
-      <c r="AO37" s="118" t="n"/>
-      <c r="AP37" s="118" t="n"/>
-      <c r="AQ37" s="118" t="n"/>
-      <c r="AR37" s="118" t="n"/>
-      <c r="AS37" s="118" t="n"/>
-      <c r="AT37" s="118" t="n"/>
-      <c r="AU37" s="118" t="n"/>
-      <c r="AV37" s="118" t="n"/>
-      <c r="AW37" s="118" t="n"/>
-      <c r="AX37" s="118" t="n"/>
-      <c r="AY37" s="118" t="n"/>
-      <c r="AZ37" s="118" t="n"/>
-      <c r="BA37" s="118" t="n"/>
-      <c r="BB37" s="118" t="n"/>
-      <c r="BC37" s="118" t="n"/>
-      <c r="BD37" s="118" t="n"/>
-      <c r="BE37" s="118" t="n"/>
-      <c r="BF37" s="118" t="n"/>
-      <c r="BG37" s="118" t="n"/>
-      <c r="BH37" s="118" t="n"/>
-      <c r="BI37" s="118" t="n"/>
-      <c r="BJ37" s="118" t="n"/>
-      <c r="BK37" s="118" t="n"/>
-      <c r="BL37" s="118" t="n"/>
-      <c r="BM37" s="118" t="n"/>
-      <c r="BN37" s="118" t="n"/>
-      <c r="BO37" s="118" t="n"/>
-      <c r="BP37" s="118" t="n"/>
-      <c r="BQ37" s="118" t="n"/>
-      <c r="BR37" s="118" t="n"/>
-      <c r="BS37" s="118" t="n"/>
-      <c r="BT37" s="118" t="n"/>
-      <c r="BU37" s="118" t="n"/>
-      <c r="BV37" s="118" t="n"/>
-      <c r="BW37" s="118" t="n"/>
-      <c r="BX37" s="118" t="n"/>
-      <c r="BY37" s="118" t="n"/>
       <c r="BZ37" s="17" t="n"/>
-      <c r="CA37" s="138" t="n"/>
-      <c r="CB37" s="139" t="n"/>
-      <c r="CC37" s="139" t="n"/>
-      <c r="CD37" s="139" t="n"/>
-      <c r="CE37" s="139" t="n"/>
-      <c r="CF37" s="139" t="n"/>
-      <c r="CG37" s="139" t="n"/>
-      <c r="CH37" s="139" t="n"/>
-      <c r="CI37" s="139" t="n"/>
-      <c r="CJ37" s="139" t="n"/>
-      <c r="CK37" s="139" t="n"/>
-      <c r="CL37" s="139" t="n"/>
-      <c r="CM37" s="139" t="n"/>
-      <c r="CN37" s="139" t="n"/>
-      <c r="CO37" s="139" t="n"/>
-      <c r="CP37" s="139" t="n"/>
-      <c r="CQ37" s="140" t="n"/>
     </row>
-    <row customHeight="1" ht="8" r="38" s="113">
+    <row customHeight="1" ht="8" r="38" s="113" spans="1:95">
       <c r="A38" s="6" t="n"/>
       <c r="B38" s="7" t="n"/>
       <c r="C38" s="7" t="n"/>
@@ -6317,75 +4603,18 @@
       <c r="AK38" s="7" t="n"/>
       <c r="AL38" s="7" t="n"/>
       <c r="AM38" s="7" t="n"/>
-      <c r="AN38" s="35" t="inlineStr">
-        <is>
-          <t>(прописью)</t>
-        </is>
-      </c>
-      <c r="AO38" s="122" t="n"/>
-      <c r="AP38" s="122" t="n"/>
-      <c r="AQ38" s="122" t="n"/>
-      <c r="AR38" s="122" t="n"/>
-      <c r="AS38" s="122" t="n"/>
-      <c r="AT38" s="122" t="n"/>
-      <c r="AU38" s="122" t="n"/>
-      <c r="AV38" s="122" t="n"/>
-      <c r="AW38" s="122" t="n"/>
-      <c r="AX38" s="122" t="n"/>
-      <c r="AY38" s="122" t="n"/>
-      <c r="AZ38" s="122" t="n"/>
-      <c r="BA38" s="122" t="n"/>
-      <c r="BB38" s="122" t="n"/>
-      <c r="BC38" s="122" t="n"/>
-      <c r="BD38" s="122" t="n"/>
-      <c r="BE38" s="122" t="n"/>
-      <c r="BF38" s="122" t="n"/>
-      <c r="BG38" s="122" t="n"/>
-      <c r="BH38" s="122" t="n"/>
-      <c r="BI38" s="122" t="n"/>
-      <c r="BJ38" s="122" t="n"/>
-      <c r="BK38" s="122" t="n"/>
-      <c r="BL38" s="122" t="n"/>
-      <c r="BM38" s="122" t="n"/>
-      <c r="BN38" s="122" t="n"/>
-      <c r="BO38" s="122" t="n"/>
-      <c r="BP38" s="122" t="n"/>
-      <c r="BQ38" s="122" t="n"/>
-      <c r="BR38" s="122" t="n"/>
-      <c r="BS38" s="122" t="n"/>
-      <c r="BT38" s="122" t="n"/>
-      <c r="BU38" s="122" t="n"/>
-      <c r="BV38" s="122" t="n"/>
-      <c r="BW38" s="122" t="n"/>
-      <c r="BX38" s="122" t="n"/>
-      <c r="BY38" s="122" t="n"/>
+      <c r="AN38" s="35" t="s">
+        <v>50</v>
+      </c>
       <c r="BZ38" s="17" t="n"/>
       <c r="CA38" s="82" t="n"/>
-      <c r="CB38" s="122" t="n"/>
-      <c r="CC38" s="122" t="n"/>
-      <c r="CD38" s="122" t="n"/>
-      <c r="CE38" s="122" t="n"/>
-      <c r="CF38" s="122" t="n"/>
-      <c r="CG38" s="122" t="n"/>
-      <c r="CH38" s="122" t="n"/>
-      <c r="CI38" s="122" t="n"/>
-      <c r="CJ38" s="122" t="n"/>
-      <c r="CK38" s="122" t="n"/>
-      <c r="CL38" s="122" t="n"/>
-      <c r="CM38" s="122" t="n"/>
-      <c r="CN38" s="122" t="n"/>
-      <c r="CO38" s="122" t="n"/>
-      <c r="CP38" s="122" t="n"/>
-      <c r="CQ38" s="124" t="n"/>
     </row>
-    <row customHeight="1" ht="15.5" r="39" s="113">
+    <row customHeight="1" ht="15.5" r="39" s="113" spans="1:95">
       <c r="A39" s="6" t="n"/>
       <c r="B39" s="7" t="n"/>
       <c r="C39" s="7" t="n"/>
-      <c r="D39" s="72" t="inlineStr">
-        <is>
-          <t>Всего мест</t>
-        </is>
+      <c r="D39" s="72" t="s">
+        <v>52</v>
       </c>
       <c r="E39" s="7" t="n"/>
       <c r="F39" s="7" t="n"/>
@@ -6394,27 +4623,9 @@
       <c r="I39" s="7" t="n"/>
       <c r="J39" s="7" t="n"/>
       <c r="K39" s="11" t="n"/>
-      <c r="L39" s="118" t="n"/>
-      <c r="M39" s="118" t="n"/>
-      <c r="N39" s="118" t="n"/>
-      <c r="O39" s="118" t="n"/>
-      <c r="P39" s="118" t="n"/>
-      <c r="Q39" s="118" t="n"/>
-      <c r="R39" s="118" t="n"/>
-      <c r="S39" s="118" t="n"/>
-      <c r="T39" s="118" t="n"/>
-      <c r="U39" s="118" t="n"/>
-      <c r="V39" s="118" t="n"/>
-      <c r="W39" s="118" t="n"/>
-      <c r="X39" s="118" t="n"/>
-      <c r="Y39" s="118" t="n"/>
-      <c r="Z39" s="118" t="n"/>
-      <c r="AA39" s="118" t="n"/>
       <c r="AB39" s="7" t="n"/>
-      <c r="AC39" s="72" t="inlineStr">
-        <is>
-          <t>Масса груза (брутто)</t>
-        </is>
+      <c r="AC39" s="72" t="s">
+        <v>53</v>
       </c>
       <c r="AD39" s="7" t="n"/>
       <c r="AE39" s="7" t="n"/>
@@ -6427,63 +4638,9 @@
       <c r="AL39" s="7" t="n"/>
       <c r="AM39" s="7" t="n"/>
       <c r="AN39" s="11" t="n"/>
-      <c r="AO39" s="118" t="n"/>
-      <c r="AP39" s="118" t="n"/>
-      <c r="AQ39" s="118" t="n"/>
-      <c r="AR39" s="118" t="n"/>
-      <c r="AS39" s="118" t="n"/>
-      <c r="AT39" s="118" t="n"/>
-      <c r="AU39" s="118" t="n"/>
-      <c r="AV39" s="118" t="n"/>
-      <c r="AW39" s="118" t="n"/>
-      <c r="AX39" s="118" t="n"/>
-      <c r="AY39" s="118" t="n"/>
-      <c r="AZ39" s="118" t="n"/>
-      <c r="BA39" s="118" t="n"/>
-      <c r="BB39" s="118" t="n"/>
-      <c r="BC39" s="118" t="n"/>
-      <c r="BD39" s="118" t="n"/>
-      <c r="BE39" s="118" t="n"/>
-      <c r="BF39" s="118" t="n"/>
-      <c r="BG39" s="118" t="n"/>
-      <c r="BH39" s="118" t="n"/>
-      <c r="BI39" s="118" t="n"/>
-      <c r="BJ39" s="118" t="n"/>
-      <c r="BK39" s="118" t="n"/>
-      <c r="BL39" s="118" t="n"/>
-      <c r="BM39" s="118" t="n"/>
-      <c r="BN39" s="118" t="n"/>
-      <c r="BO39" s="118" t="n"/>
-      <c r="BP39" s="118" t="n"/>
-      <c r="BQ39" s="118" t="n"/>
-      <c r="BR39" s="118" t="n"/>
-      <c r="BS39" s="118" t="n"/>
-      <c r="BT39" s="118" t="n"/>
-      <c r="BU39" s="118" t="n"/>
-      <c r="BV39" s="118" t="n"/>
-      <c r="BW39" s="118" t="n"/>
-      <c r="BX39" s="118" t="n"/>
-      <c r="BY39" s="118" t="n"/>
       <c r="BZ39" s="17" t="n"/>
-      <c r="CA39" s="125" t="n"/>
-      <c r="CB39" s="118" t="n"/>
-      <c r="CC39" s="118" t="n"/>
-      <c r="CD39" s="118" t="n"/>
-      <c r="CE39" s="118" t="n"/>
-      <c r="CF39" s="118" t="n"/>
-      <c r="CG39" s="118" t="n"/>
-      <c r="CH39" s="118" t="n"/>
-      <c r="CI39" s="118" t="n"/>
-      <c r="CJ39" s="118" t="n"/>
-      <c r="CK39" s="118" t="n"/>
-      <c r="CL39" s="118" t="n"/>
-      <c r="CM39" s="118" t="n"/>
-      <c r="CN39" s="118" t="n"/>
-      <c r="CO39" s="118" t="n"/>
-      <c r="CP39" s="118" t="n"/>
-      <c r="CQ39" s="126" t="n"/>
     </row>
-    <row customHeight="1" ht="8" r="40" s="113">
+    <row customHeight="1" ht="8" r="40" s="113" spans="1:95">
       <c r="A40" s="6" t="n"/>
       <c r="B40" s="7" t="n"/>
       <c r="C40" s="7" t="n"/>
@@ -6494,27 +4651,9 @@
       <c r="H40" s="7" t="n"/>
       <c r="I40" s="7" t="n"/>
       <c r="J40" s="7" t="n"/>
-      <c r="K40" s="35" t="inlineStr">
-        <is>
-          <t>(прописью)</t>
-        </is>
-      </c>
-      <c r="L40" s="122" t="n"/>
-      <c r="M40" s="122" t="n"/>
-      <c r="N40" s="122" t="n"/>
-      <c r="O40" s="122" t="n"/>
-      <c r="P40" s="122" t="n"/>
-      <c r="Q40" s="122" t="n"/>
-      <c r="R40" s="122" t="n"/>
-      <c r="S40" s="122" t="n"/>
-      <c r="T40" s="122" t="n"/>
-      <c r="U40" s="122" t="n"/>
-      <c r="V40" s="122" t="n"/>
-      <c r="W40" s="122" t="n"/>
-      <c r="X40" s="122" t="n"/>
-      <c r="Y40" s="122" t="n"/>
-      <c r="Z40" s="122" t="n"/>
-      <c r="AA40" s="122" t="n"/>
+      <c r="K40" s="35" t="s">
+        <v>50</v>
+      </c>
       <c r="AB40" s="75" t="n"/>
       <c r="AC40" s="7" t="n"/>
       <c r="AD40" s="7" t="n"/>
@@ -6527,48 +4666,9 @@
       <c r="AK40" s="7" t="n"/>
       <c r="AL40" s="7" t="n"/>
       <c r="AM40" s="7" t="n"/>
-      <c r="AN40" s="35" t="inlineStr">
-        <is>
-          <t>(прописью)</t>
-        </is>
-      </c>
-      <c r="AO40" s="122" t="n"/>
-      <c r="AP40" s="122" t="n"/>
-      <c r="AQ40" s="122" t="n"/>
-      <c r="AR40" s="122" t="n"/>
-      <c r="AS40" s="122" t="n"/>
-      <c r="AT40" s="122" t="n"/>
-      <c r="AU40" s="122" t="n"/>
-      <c r="AV40" s="122" t="n"/>
-      <c r="AW40" s="122" t="n"/>
-      <c r="AX40" s="122" t="n"/>
-      <c r="AY40" s="122" t="n"/>
-      <c r="AZ40" s="122" t="n"/>
-      <c r="BA40" s="122" t="n"/>
-      <c r="BB40" s="122" t="n"/>
-      <c r="BC40" s="122" t="n"/>
-      <c r="BD40" s="122" t="n"/>
-      <c r="BE40" s="122" t="n"/>
-      <c r="BF40" s="122" t="n"/>
-      <c r="BG40" s="122" t="n"/>
-      <c r="BH40" s="122" t="n"/>
-      <c r="BI40" s="122" t="n"/>
-      <c r="BJ40" s="122" t="n"/>
-      <c r="BK40" s="122" t="n"/>
-      <c r="BL40" s="122" t="n"/>
-      <c r="BM40" s="122" t="n"/>
-      <c r="BN40" s="122" t="n"/>
-      <c r="BO40" s="122" t="n"/>
-      <c r="BP40" s="122" t="n"/>
-      <c r="BQ40" s="122" t="n"/>
-      <c r="BR40" s="122" t="n"/>
-      <c r="BS40" s="122" t="n"/>
-      <c r="BT40" s="122" t="n"/>
-      <c r="BU40" s="122" t="n"/>
-      <c r="BV40" s="122" t="n"/>
-      <c r="BW40" s="122" t="n"/>
-      <c r="BX40" s="122" t="n"/>
-      <c r="BY40" s="122" t="n"/>
+      <c r="AN40" s="35" t="s">
+        <v>50</v>
+      </c>
       <c r="BZ40" s="7" t="n"/>
       <c r="CA40" s="52" t="n"/>
       <c r="CB40" s="52" t="n"/>
@@ -6588,7 +4688,7 @@
       <c r="CP40" s="52" t="n"/>
       <c r="CQ40" s="53" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="41" s="113">
+    <row customHeight="1" ht="15" r="41" s="113" spans="1:95">
       <c r="A41" s="6" t="n"/>
       <c r="B41" s="7" t="n"/>
       <c r="C41" s="7" t="n"/>
@@ -6685,11 +4785,9 @@
       <c r="CP41" s="7" t="n"/>
       <c r="CQ41" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="42" s="113">
-      <c r="A42" s="86" t="inlineStr">
-        <is>
-          <t>Приложение (паспорта, сертификаты и т.п.) на</t>
-        </is>
+    <row customHeight="1" ht="15" r="42" s="113" spans="1:95">
+      <c r="A42" s="86" t="s">
+        <v>54</v>
       </c>
       <c r="B42" s="7" t="n"/>
       <c r="C42" s="7" t="n"/>
@@ -6714,39 +4812,16 @@
       <c r="V42" s="7" t="n"/>
       <c r="W42" s="7" t="n"/>
       <c r="X42" s="87" t="n"/>
-      <c r="Y42" s="118" t="n"/>
-      <c r="Z42" s="118" t="n"/>
-      <c r="AA42" s="118" t="n"/>
-      <c r="AB42" s="118" t="n"/>
-      <c r="AC42" s="118" t="n"/>
-      <c r="AD42" s="118" t="n"/>
-      <c r="AE42" s="118" t="n"/>
-      <c r="AF42" s="118" t="n"/>
-      <c r="AG42" s="118" t="n"/>
-      <c r="AH42" s="118" t="n"/>
-      <c r="AI42" s="118" t="n"/>
-      <c r="AJ42" s="118" t="n"/>
-      <c r="AK42" s="118" t="n"/>
-      <c r="AL42" s="118" t="n"/>
-      <c r="AM42" s="118" t="n"/>
-      <c r="AN42" s="118" t="n"/>
-      <c r="AO42" s="118" t="n"/>
-      <c r="AP42" s="118" t="n"/>
-      <c r="AQ42" s="118" t="n"/>
       <c r="AR42" s="7" t="n"/>
-      <c r="AS42" s="72" t="inlineStr">
-        <is>
-          <t>листах</t>
-        </is>
+      <c r="AS42" s="72" t="s">
+        <v>55</v>
       </c>
       <c r="AT42" s="7" t="n"/>
       <c r="AU42" s="7" t="n"/>
       <c r="AV42" s="88" t="n"/>
       <c r="AW42" s="55" t="n"/>
-      <c r="AX42" s="72" t="inlineStr">
-        <is>
-          <t>По доверенности №</t>
-        </is>
+      <c r="AX42" s="72" t="s">
+        <v>56</v>
       </c>
       <c r="AY42" s="7" t="n"/>
       <c r="AZ42" s="7" t="n"/>
@@ -6758,55 +4833,24 @@
       <c r="BF42" s="7" t="n"/>
       <c r="BG42" s="7" t="n"/>
       <c r="BH42" s="87" t="n"/>
-      <c r="BI42" s="118" t="n"/>
-      <c r="BJ42" s="118" t="n"/>
-      <c r="BK42" s="118" t="n"/>
-      <c r="BL42" s="118" t="n"/>
-      <c r="BM42" s="118" t="n"/>
-      <c r="BN42" s="118" t="n"/>
-      <c r="BO42" s="118" t="n"/>
-      <c r="BP42" s="118" t="n"/>
-      <c r="BQ42" s="118" t="n"/>
-      <c r="BR42" s="118" t="n"/>
-      <c r="BS42" s="118" t="n"/>
-      <c r="BT42" s="118" t="n"/>
-      <c r="BU42" s="118" t="n"/>
       <c r="BV42" s="7" t="n"/>
       <c r="BW42" s="7" t="n"/>
-      <c r="BX42" s="89" t="inlineStr">
-        <is>
-          <t>от  «</t>
-        </is>
+      <c r="BX42" s="89" t="s">
+        <v>57</v>
       </c>
       <c r="BY42" s="87" t="n"/>
-      <c r="BZ42" s="118" t="n"/>
-      <c r="CA42" s="90" t="inlineStr">
-        <is>
-          <t>»</t>
-        </is>
+      <c r="CA42" s="90" t="s">
+        <v>58</v>
       </c>
       <c r="CB42" s="7" t="n"/>
       <c r="CC42" s="87" t="n"/>
-      <c r="CD42" s="118" t="n"/>
-      <c r="CE42" s="118" t="n"/>
-      <c r="CF42" s="118" t="n"/>
-      <c r="CG42" s="118" t="n"/>
-      <c r="CH42" s="118" t="n"/>
-      <c r="CI42" s="118" t="n"/>
-      <c r="CJ42" s="118" t="n"/>
       <c r="CK42" s="90" t="n"/>
       <c r="CL42" s="87" t="n"/>
-      <c r="CM42" s="118" t="n"/>
-      <c r="CN42" s="118" t="n"/>
-      <c r="CO42" s="92" t="inlineStr">
-        <is>
-          <t>года,</t>
-        </is>
-      </c>
-      <c r="CP42" s="141" t="n"/>
-      <c r="CQ42" s="142" t="n"/>
+      <c r="CO42" s="91" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row customHeight="1" ht="8" r="43" s="113">
+    <row customHeight="1" ht="8" r="43" s="113" spans="1:95">
       <c r="A43" s="6" t="n"/>
       <c r="B43" s="7" t="n"/>
       <c r="C43" s="7" t="n"/>
@@ -6830,30 +4874,9 @@
       <c r="U43" s="7" t="n"/>
       <c r="V43" s="7" t="n"/>
       <c r="W43" s="7" t="n"/>
-      <c r="X43" s="35" t="inlineStr">
-        <is>
-          <t>(прописью)</t>
-        </is>
-      </c>
-      <c r="Y43" s="122" t="n"/>
-      <c r="Z43" s="122" t="n"/>
-      <c r="AA43" s="122" t="n"/>
-      <c r="AB43" s="122" t="n"/>
-      <c r="AC43" s="122" t="n"/>
-      <c r="AD43" s="122" t="n"/>
-      <c r="AE43" s="122" t="n"/>
-      <c r="AF43" s="122" t="n"/>
-      <c r="AG43" s="122" t="n"/>
-      <c r="AH43" s="122" t="n"/>
-      <c r="AI43" s="122" t="n"/>
-      <c r="AJ43" s="122" t="n"/>
-      <c r="AK43" s="122" t="n"/>
-      <c r="AL43" s="122" t="n"/>
-      <c r="AM43" s="122" t="n"/>
-      <c r="AN43" s="122" t="n"/>
-      <c r="AO43" s="122" t="n"/>
-      <c r="AP43" s="122" t="n"/>
-      <c r="AQ43" s="122" t="n"/>
+      <c r="X43" s="35" t="s">
+        <v>50</v>
+      </c>
       <c r="AR43" s="7" t="n"/>
       <c r="AS43" s="7" t="n"/>
       <c r="AT43" s="7" t="n"/>
@@ -6907,11 +4930,9 @@
       <c r="CP43" s="7" t="n"/>
       <c r="CQ43" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="44" s="113">
-      <c r="A44" s="86" t="inlineStr">
-        <is>
-          <t>Всего отпущено на сумму</t>
-        </is>
+    <row customHeight="1" ht="15" r="44" s="113" spans="1:95">
+      <c r="A44" s="86" t="s">
+        <v>60</v>
       </c>
       <c r="B44" s="7" t="n"/>
       <c r="C44" s="7" t="n"/>
@@ -6926,93 +4947,21 @@
       <c r="L44" s="7" t="n"/>
       <c r="M44" s="7" t="n"/>
       <c r="N44" s="87" t="n"/>
-      <c r="O44" s="118" t="n"/>
-      <c r="P44" s="118" t="n"/>
-      <c r="Q44" s="118" t="n"/>
-      <c r="R44" s="118" t="n"/>
-      <c r="S44" s="118" t="n"/>
-      <c r="T44" s="118" t="n"/>
-      <c r="U44" s="118" t="n"/>
-      <c r="V44" s="118" t="n"/>
-      <c r="W44" s="118" t="n"/>
-      <c r="X44" s="118" t="n"/>
-      <c r="Y44" s="118" t="n"/>
-      <c r="Z44" s="118" t="n"/>
-      <c r="AA44" s="118" t="n"/>
-      <c r="AB44" s="118" t="n"/>
-      <c r="AC44" s="118" t="n"/>
-      <c r="AD44" s="118" t="n"/>
-      <c r="AE44" s="118" t="n"/>
-      <c r="AF44" s="118" t="n"/>
-      <c r="AG44" s="118" t="n"/>
-      <c r="AH44" s="118" t="n"/>
-      <c r="AI44" s="118" t="n"/>
-      <c r="AJ44" s="118" t="n"/>
-      <c r="AK44" s="118" t="n"/>
-      <c r="AL44" s="118" t="n"/>
-      <c r="AM44" s="118" t="n"/>
-      <c r="AN44" s="118" t="n"/>
-      <c r="AO44" s="118" t="n"/>
-      <c r="AP44" s="118" t="n"/>
-      <c r="AQ44" s="118" t="n"/>
-      <c r="AR44" s="118" t="n"/>
-      <c r="AS44" s="118" t="n"/>
       <c r="AT44" s="7" t="n"/>
       <c r="AU44" s="7" t="n"/>
       <c r="AV44" s="88" t="n"/>
       <c r="AW44" s="55" t="n"/>
-      <c r="AX44" s="72" t="inlineStr">
-        <is>
-          <t>выданной</t>
-        </is>
+      <c r="AX44" s="72" t="s">
+        <v>61</v>
       </c>
       <c r="AY44" s="7" t="n"/>
       <c r="AZ44" s="7" t="n"/>
       <c r="BA44" s="7" t="n"/>
       <c r="BB44" s="7" t="n"/>
       <c r="BC44" s="7" t="n"/>
-      <c r="BD44" s="94" t="n"/>
-      <c r="BE44" s="118" t="n"/>
-      <c r="BF44" s="118" t="n"/>
-      <c r="BG44" s="118" t="n"/>
-      <c r="BH44" s="118" t="n"/>
-      <c r="BI44" s="118" t="n"/>
-      <c r="BJ44" s="118" t="n"/>
-      <c r="BK44" s="118" t="n"/>
-      <c r="BL44" s="118" t="n"/>
-      <c r="BM44" s="118" t="n"/>
-      <c r="BN44" s="118" t="n"/>
-      <c r="BO44" s="118" t="n"/>
-      <c r="BP44" s="118" t="n"/>
-      <c r="BQ44" s="118" t="n"/>
-      <c r="BR44" s="118" t="n"/>
-      <c r="BS44" s="118" t="n"/>
-      <c r="BT44" s="118" t="n"/>
-      <c r="BU44" s="118" t="n"/>
-      <c r="BV44" s="118" t="n"/>
-      <c r="BW44" s="118" t="n"/>
-      <c r="BX44" s="118" t="n"/>
-      <c r="BY44" s="118" t="n"/>
-      <c r="BZ44" s="118" t="n"/>
-      <c r="CA44" s="118" t="n"/>
-      <c r="CB44" s="118" t="n"/>
-      <c r="CC44" s="118" t="n"/>
-      <c r="CD44" s="118" t="n"/>
-      <c r="CE44" s="118" t="n"/>
-      <c r="CF44" s="118" t="n"/>
-      <c r="CG44" s="118" t="n"/>
-      <c r="CH44" s="118" t="n"/>
-      <c r="CI44" s="118" t="n"/>
-      <c r="CJ44" s="118" t="n"/>
-      <c r="CK44" s="118" t="n"/>
-      <c r="CL44" s="118" t="n"/>
-      <c r="CM44" s="118" t="n"/>
-      <c r="CN44" s="118" t="n"/>
-      <c r="CO44" s="118" t="n"/>
-      <c r="CP44" s="118" t="n"/>
-      <c r="CQ44" s="143" t="n"/>
+      <c r="BD44" s="93" t="n"/>
     </row>
-    <row customHeight="1" ht="8" r="45" s="113">
+    <row customHeight="1" ht="8" r="45" s="113" spans="1:95">
       <c r="A45" s="6" t="n"/>
       <c r="B45" s="7" t="n"/>
       <c r="C45" s="7" t="n"/>
@@ -7026,42 +4975,9 @@
       <c r="K45" s="7" t="n"/>
       <c r="L45" s="7" t="n"/>
       <c r="M45" s="7" t="n"/>
-      <c r="N45" s="35" t="inlineStr">
-        <is>
-          <t>(прописью)</t>
-        </is>
-      </c>
-      <c r="O45" s="122" t="n"/>
-      <c r="P45" s="122" t="n"/>
-      <c r="Q45" s="122" t="n"/>
-      <c r="R45" s="122" t="n"/>
-      <c r="S45" s="122" t="n"/>
-      <c r="T45" s="122" t="n"/>
-      <c r="U45" s="122" t="n"/>
-      <c r="V45" s="122" t="n"/>
-      <c r="W45" s="122" t="n"/>
-      <c r="X45" s="122" t="n"/>
-      <c r="Y45" s="122" t="n"/>
-      <c r="Z45" s="122" t="n"/>
-      <c r="AA45" s="122" t="n"/>
-      <c r="AB45" s="122" t="n"/>
-      <c r="AC45" s="122" t="n"/>
-      <c r="AD45" s="122" t="n"/>
-      <c r="AE45" s="122" t="n"/>
-      <c r="AF45" s="122" t="n"/>
-      <c r="AG45" s="122" t="n"/>
-      <c r="AH45" s="122" t="n"/>
-      <c r="AI45" s="122" t="n"/>
-      <c r="AJ45" s="122" t="n"/>
-      <c r="AK45" s="122" t="n"/>
-      <c r="AL45" s="122" t="n"/>
-      <c r="AM45" s="122" t="n"/>
-      <c r="AN45" s="122" t="n"/>
-      <c r="AO45" s="122" t="n"/>
-      <c r="AP45" s="122" t="n"/>
-      <c r="AQ45" s="122" t="n"/>
-      <c r="AR45" s="122" t="n"/>
-      <c r="AS45" s="122" t="n"/>
+      <c r="N45" s="35" t="s">
+        <v>50</v>
+      </c>
       <c r="AT45" s="7" t="n"/>
       <c r="AU45" s="7" t="n"/>
       <c r="AV45" s="88" t="n"/>
@@ -7072,157 +4988,23 @@
       <c r="BA45" s="7" t="n"/>
       <c r="BB45" s="7" t="n"/>
       <c r="BC45" s="7" t="n"/>
-      <c r="BD45" s="95" t="inlineStr">
-        <is>
-          <t>(кем, кому (организация, должность, фамилия, и., о.))</t>
-        </is>
-      </c>
-      <c r="BE45" s="122" t="n"/>
-      <c r="BF45" s="122" t="n"/>
-      <c r="BG45" s="122" t="n"/>
-      <c r="BH45" s="122" t="n"/>
-      <c r="BI45" s="122" t="n"/>
-      <c r="BJ45" s="122" t="n"/>
-      <c r="BK45" s="122" t="n"/>
-      <c r="BL45" s="122" t="n"/>
-      <c r="BM45" s="122" t="n"/>
-      <c r="BN45" s="122" t="n"/>
-      <c r="BO45" s="122" t="n"/>
-      <c r="BP45" s="122" t="n"/>
-      <c r="BQ45" s="122" t="n"/>
-      <c r="BR45" s="122" t="n"/>
-      <c r="BS45" s="122" t="n"/>
-      <c r="BT45" s="122" t="n"/>
-      <c r="BU45" s="122" t="n"/>
-      <c r="BV45" s="122" t="n"/>
-      <c r="BW45" s="122" t="n"/>
-      <c r="BX45" s="122" t="n"/>
-      <c r="BY45" s="122" t="n"/>
-      <c r="BZ45" s="122" t="n"/>
-      <c r="CA45" s="122" t="n"/>
-      <c r="CB45" s="122" t="n"/>
-      <c r="CC45" s="122" t="n"/>
-      <c r="CD45" s="122" t="n"/>
-      <c r="CE45" s="122" t="n"/>
-      <c r="CF45" s="122" t="n"/>
-      <c r="CG45" s="122" t="n"/>
-      <c r="CH45" s="122" t="n"/>
-      <c r="CI45" s="122" t="n"/>
-      <c r="CJ45" s="122" t="n"/>
-      <c r="CK45" s="122" t="n"/>
-      <c r="CL45" s="122" t="n"/>
-      <c r="CM45" s="122" t="n"/>
-      <c r="CN45" s="122" t="n"/>
-      <c r="CO45" s="122" t="n"/>
-      <c r="CP45" s="122" t="n"/>
-      <c r="CQ45" s="144" t="n"/>
+      <c r="BD45" s="35" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row customHeight="1" ht="15.75" r="46" s="113">
+    <row customHeight="1" ht="15.75" r="46" s="113" spans="1:95">
       <c r="A46" s="96" t="n"/>
-      <c r="B46" s="118" t="n"/>
-      <c r="C46" s="118" t="n"/>
-      <c r="D46" s="118" t="n"/>
-      <c r="E46" s="118" t="n"/>
-      <c r="F46" s="118" t="n"/>
-      <c r="G46" s="118" t="n"/>
-      <c r="H46" s="118" t="n"/>
-      <c r="I46" s="118" t="n"/>
-      <c r="J46" s="118" t="n"/>
-      <c r="K46" s="118" t="n"/>
-      <c r="L46" s="118" t="n"/>
-      <c r="M46" s="118" t="n"/>
-      <c r="N46" s="118" t="n"/>
-      <c r="O46" s="118" t="n"/>
-      <c r="P46" s="118" t="n"/>
-      <c r="Q46" s="118" t="n"/>
-      <c r="R46" s="118" t="n"/>
-      <c r="S46" s="118" t="n"/>
-      <c r="T46" s="118" t="n"/>
-      <c r="U46" s="118" t="n"/>
-      <c r="V46" s="118" t="n"/>
-      <c r="W46" s="118" t="n"/>
-      <c r="X46" s="118" t="n"/>
-      <c r="Y46" s="118" t="n"/>
-      <c r="Z46" s="118" t="n"/>
-      <c r="AA46" s="118" t="n"/>
-      <c r="AB46" s="118" t="n"/>
-      <c r="AC46" s="118" t="n"/>
-      <c r="AD46" s="118" t="n"/>
-      <c r="AE46" s="118" t="n"/>
-      <c r="AF46" s="118" t="n"/>
-      <c r="AG46" s="118" t="n"/>
-      <c r="AH46" s="118" t="n"/>
-      <c r="AI46" s="119" t="n"/>
-      <c r="AJ46" s="91" t="inlineStr">
-        <is>
-          <t>руб.</t>
-        </is>
-      </c>
-      <c r="AK46" s="141" t="n"/>
-      <c r="AL46" s="141" t="n"/>
+      <c r="AJ46" s="91" t="s">
+        <v>63</v>
+      </c>
       <c r="AM46" s="87" t="n"/>
-      <c r="AN46" s="118" t="n"/>
-      <c r="AO46" s="118" t="n"/>
-      <c r="AP46" s="118" t="n"/>
-      <c r="AQ46" s="118" t="n"/>
-      <c r="AR46" s="118" t="n"/>
-      <c r="AS46" s="118" t="n"/>
-      <c r="AT46" s="98" t="inlineStr">
-        <is>
-          <t>коп.</t>
-        </is>
-      </c>
-      <c r="AU46" s="141" t="n"/>
-      <c r="AV46" s="145" t="n"/>
+      <c r="AT46" s="91" t="s">
+        <v>64</v>
+      </c>
       <c r="AW46" s="99" t="n"/>
-      <c r="AX46" s="94" t="n"/>
-      <c r="AY46" s="118" t="n"/>
-      <c r="AZ46" s="118" t="n"/>
-      <c r="BA46" s="118" t="n"/>
-      <c r="BB46" s="118" t="n"/>
-      <c r="BC46" s="118" t="n"/>
-      <c r="BD46" s="118" t="n"/>
-      <c r="BE46" s="118" t="n"/>
-      <c r="BF46" s="118" t="n"/>
-      <c r="BG46" s="118" t="n"/>
-      <c r="BH46" s="118" t="n"/>
-      <c r="BI46" s="118" t="n"/>
-      <c r="BJ46" s="118" t="n"/>
-      <c r="BK46" s="118" t="n"/>
-      <c r="BL46" s="118" t="n"/>
-      <c r="BM46" s="118" t="n"/>
-      <c r="BN46" s="118" t="n"/>
-      <c r="BO46" s="118" t="n"/>
-      <c r="BP46" s="118" t="n"/>
-      <c r="BQ46" s="118" t="n"/>
-      <c r="BR46" s="118" t="n"/>
-      <c r="BS46" s="118" t="n"/>
-      <c r="BT46" s="118" t="n"/>
-      <c r="BU46" s="118" t="n"/>
-      <c r="BV46" s="118" t="n"/>
-      <c r="BW46" s="118" t="n"/>
-      <c r="BX46" s="118" t="n"/>
-      <c r="BY46" s="118" t="n"/>
-      <c r="BZ46" s="118" t="n"/>
-      <c r="CA46" s="118" t="n"/>
-      <c r="CB46" s="118" t="n"/>
-      <c r="CC46" s="118" t="n"/>
-      <c r="CD46" s="118" t="n"/>
-      <c r="CE46" s="118" t="n"/>
-      <c r="CF46" s="118" t="n"/>
-      <c r="CG46" s="118" t="n"/>
-      <c r="CH46" s="118" t="n"/>
-      <c r="CI46" s="118" t="n"/>
-      <c r="CJ46" s="118" t="n"/>
-      <c r="CK46" s="118" t="n"/>
-      <c r="CL46" s="118" t="n"/>
-      <c r="CM46" s="118" t="n"/>
-      <c r="CN46" s="118" t="n"/>
-      <c r="CO46" s="118" t="n"/>
-      <c r="CP46" s="118" t="n"/>
-      <c r="CQ46" s="143" t="n"/>
+      <c r="AX46" s="93" t="n"/>
     </row>
-    <row customHeight="1" ht="8.25" r="47" s="113">
+    <row customHeight="1" ht="8.25" r="47" s="113" spans="1:95">
       <c r="A47" s="70" t="n"/>
       <c r="B47" s="26" t="n"/>
       <c r="C47" s="26" t="n"/>
@@ -7319,11 +5101,9 @@
       <c r="CP47" s="26" t="n"/>
       <c r="CQ47" s="100" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="48" s="113">
-      <c r="A48" s="86" t="inlineStr">
-        <is>
-          <t>Отпуск груза разрешил</t>
-        </is>
+    <row customHeight="1" ht="15" r="48" s="113" spans="1:95">
+      <c r="A48" s="86" t="s">
+        <v>65</v>
       </c>
       <c r="B48" s="7" t="n"/>
       <c r="C48" s="7" t="n"/>
@@ -7336,91 +5116,15 @@
       <c r="J48" s="7" t="n"/>
       <c r="K48" s="91" t="n"/>
       <c r="L48" s="87" t="n"/>
-      <c r="M48" s="118" t="n"/>
-      <c r="N48" s="118" t="n"/>
-      <c r="O48" s="118" t="n"/>
-      <c r="P48" s="118" t="n"/>
-      <c r="Q48" s="118" t="n"/>
-      <c r="R48" s="118" t="n"/>
-      <c r="S48" s="118" t="n"/>
-      <c r="T48" s="118" t="n"/>
       <c r="U48" s="91" t="n"/>
       <c r="V48" s="87" t="n"/>
-      <c r="W48" s="118" t="n"/>
-      <c r="X48" s="118" t="n"/>
-      <c r="Y48" s="118" t="n"/>
-      <c r="Z48" s="118" t="n"/>
-      <c r="AA48" s="118" t="n"/>
-      <c r="AB48" s="118" t="n"/>
-      <c r="AC48" s="118" t="n"/>
-      <c r="AD48" s="118" t="n"/>
-      <c r="AE48" s="118" t="n"/>
       <c r="AF48" s="91" t="n"/>
       <c r="AG48" s="87" t="n"/>
-      <c r="AH48" s="118" t="n"/>
-      <c r="AI48" s="118" t="n"/>
-      <c r="AJ48" s="118" t="n"/>
-      <c r="AK48" s="118" t="n"/>
-      <c r="AL48" s="118" t="n"/>
-      <c r="AM48" s="118" t="n"/>
-      <c r="AN48" s="118" t="n"/>
-      <c r="AO48" s="118" t="n"/>
-      <c r="AP48" s="118" t="n"/>
-      <c r="AQ48" s="118" t="n"/>
-      <c r="AR48" s="118" t="n"/>
-      <c r="AS48" s="118" t="n"/>
-      <c r="AT48" s="118" t="n"/>
-      <c r="AU48" s="118" t="n"/>
       <c r="AV48" s="88" t="n"/>
       <c r="AW48" s="99" t="n"/>
-      <c r="AX48" s="94" t="n"/>
-      <c r="AY48" s="118" t="n"/>
-      <c r="AZ48" s="118" t="n"/>
-      <c r="BA48" s="118" t="n"/>
-      <c r="BB48" s="118" t="n"/>
-      <c r="BC48" s="118" t="n"/>
-      <c r="BD48" s="118" t="n"/>
-      <c r="BE48" s="118" t="n"/>
-      <c r="BF48" s="118" t="n"/>
-      <c r="BG48" s="118" t="n"/>
-      <c r="BH48" s="118" t="n"/>
-      <c r="BI48" s="118" t="n"/>
-      <c r="BJ48" s="118" t="n"/>
-      <c r="BK48" s="118" t="n"/>
-      <c r="BL48" s="118" t="n"/>
-      <c r="BM48" s="118" t="n"/>
-      <c r="BN48" s="118" t="n"/>
-      <c r="BO48" s="118" t="n"/>
-      <c r="BP48" s="118" t="n"/>
-      <c r="BQ48" s="118" t="n"/>
-      <c r="BR48" s="118" t="n"/>
-      <c r="BS48" s="118" t="n"/>
-      <c r="BT48" s="118" t="n"/>
-      <c r="BU48" s="118" t="n"/>
-      <c r="BV48" s="118" t="n"/>
-      <c r="BW48" s="118" t="n"/>
-      <c r="BX48" s="118" t="n"/>
-      <c r="BY48" s="118" t="n"/>
-      <c r="BZ48" s="118" t="n"/>
-      <c r="CA48" s="118" t="n"/>
-      <c r="CB48" s="118" t="n"/>
-      <c r="CC48" s="118" t="n"/>
-      <c r="CD48" s="118" t="n"/>
-      <c r="CE48" s="118" t="n"/>
-      <c r="CF48" s="118" t="n"/>
-      <c r="CG48" s="118" t="n"/>
-      <c r="CH48" s="118" t="n"/>
-      <c r="CI48" s="118" t="n"/>
-      <c r="CJ48" s="118" t="n"/>
-      <c r="CK48" s="118" t="n"/>
-      <c r="CL48" s="118" t="n"/>
-      <c r="CM48" s="118" t="n"/>
-      <c r="CN48" s="118" t="n"/>
-      <c r="CO48" s="118" t="n"/>
-      <c r="CP48" s="118" t="n"/>
-      <c r="CQ48" s="143" t="n"/>
+      <c r="AX48" s="93" t="n"/>
     </row>
-    <row customHeight="1" ht="8" r="49" s="113">
+    <row customHeight="1" ht="8" r="49" s="113" spans="1:95">
       <c r="A49" s="6" t="n"/>
       <c r="B49" s="7" t="n"/>
       <c r="C49" s="7" t="n"/>
@@ -7432,54 +5136,17 @@
       <c r="I49" s="7" t="n"/>
       <c r="J49" s="7" t="n"/>
       <c r="K49" s="101" t="n"/>
-      <c r="L49" s="35" t="inlineStr">
-        <is>
-          <t>(должность)</t>
-        </is>
-      </c>
-      <c r="M49" s="122" t="n"/>
-      <c r="N49" s="122" t="n"/>
-      <c r="O49" s="122" t="n"/>
-      <c r="P49" s="122" t="n"/>
-      <c r="Q49" s="122" t="n"/>
-      <c r="R49" s="122" t="n"/>
-      <c r="S49" s="122" t="n"/>
-      <c r="T49" s="122" t="n"/>
+      <c r="L49" s="35" t="s">
+        <v>66</v>
+      </c>
       <c r="U49" s="7" t="n"/>
-      <c r="V49" s="35" t="inlineStr">
-        <is>
-          <t>(подпись)</t>
-        </is>
-      </c>
-      <c r="W49" s="122" t="n"/>
-      <c r="X49" s="122" t="n"/>
-      <c r="Y49" s="122" t="n"/>
-      <c r="Z49" s="122" t="n"/>
-      <c r="AA49" s="122" t="n"/>
-      <c r="AB49" s="122" t="n"/>
-      <c r="AC49" s="122" t="n"/>
-      <c r="AD49" s="122" t="n"/>
-      <c r="AE49" s="122" t="n"/>
+      <c r="V49" s="35" t="s">
+        <v>67</v>
+      </c>
       <c r="AF49" s="91" t="n"/>
-      <c r="AG49" s="35" t="inlineStr">
-        <is>
-          <t>(расшифровка подписи)</t>
-        </is>
-      </c>
-      <c r="AH49" s="122" t="n"/>
-      <c r="AI49" s="122" t="n"/>
-      <c r="AJ49" s="122" t="n"/>
-      <c r="AK49" s="122" t="n"/>
-      <c r="AL49" s="122" t="n"/>
-      <c r="AM49" s="122" t="n"/>
-      <c r="AN49" s="122" t="n"/>
-      <c r="AO49" s="122" t="n"/>
-      <c r="AP49" s="122" t="n"/>
-      <c r="AQ49" s="122" t="n"/>
-      <c r="AR49" s="122" t="n"/>
-      <c r="AS49" s="122" t="n"/>
-      <c r="AT49" s="122" t="n"/>
-      <c r="AU49" s="122" t="n"/>
+      <c r="AG49" s="35" t="s">
+        <v>68</v>
+      </c>
       <c r="AV49" s="88" t="n"/>
       <c r="AW49" s="55" t="n"/>
       <c r="AX49" s="26" t="n"/>
@@ -7529,11 +5196,9 @@
       <c r="CP49" s="26" t="n"/>
       <c r="CQ49" s="100" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="50" s="113">
-      <c r="A50" s="86" t="inlineStr">
-        <is>
-          <t>Главный (старший) бухгалтер</t>
-        </is>
+    <row customHeight="1" ht="15" r="50" s="113" spans="1:95">
+      <c r="A50" s="86" t="s">
+        <v>69</v>
       </c>
       <c r="B50" s="7" t="n"/>
       <c r="C50" s="7" t="n"/>
@@ -7556,37 +5221,12 @@
       <c r="T50" s="7" t="n"/>
       <c r="U50" s="7" t="n"/>
       <c r="V50" s="87" t="n"/>
-      <c r="W50" s="118" t="n"/>
-      <c r="X50" s="118" t="n"/>
-      <c r="Y50" s="118" t="n"/>
-      <c r="Z50" s="118" t="n"/>
-      <c r="AA50" s="118" t="n"/>
-      <c r="AB50" s="118" t="n"/>
-      <c r="AC50" s="118" t="n"/>
-      <c r="AD50" s="118" t="n"/>
-      <c r="AE50" s="118" t="n"/>
       <c r="AF50" s="91" t="n"/>
       <c r="AG50" s="87" t="n"/>
-      <c r="AH50" s="118" t="n"/>
-      <c r="AI50" s="118" t="n"/>
-      <c r="AJ50" s="118" t="n"/>
-      <c r="AK50" s="118" t="n"/>
-      <c r="AL50" s="118" t="n"/>
-      <c r="AM50" s="118" t="n"/>
-      <c r="AN50" s="118" t="n"/>
-      <c r="AO50" s="118" t="n"/>
-      <c r="AP50" s="118" t="n"/>
-      <c r="AQ50" s="118" t="n"/>
-      <c r="AR50" s="118" t="n"/>
-      <c r="AS50" s="118" t="n"/>
-      <c r="AT50" s="118" t="n"/>
-      <c r="AU50" s="118" t="n"/>
       <c r="AV50" s="88" t="n"/>
       <c r="AW50" s="55" t="n"/>
-      <c r="AX50" s="72" t="inlineStr">
-        <is>
-          <t>Груз принял</t>
-        </is>
+      <c r="AX50" s="72" t="s">
+        <v>70</v>
       </c>
       <c r="AY50" s="7" t="n"/>
       <c r="AZ50" s="7" t="n"/>
@@ -7595,46 +5235,12 @@
       <c r="BC50" s="7" t="n"/>
       <c r="BD50" s="7" t="n"/>
       <c r="BE50" s="87" t="n"/>
-      <c r="BF50" s="118" t="n"/>
-      <c r="BG50" s="118" t="n"/>
-      <c r="BH50" s="118" t="n"/>
-      <c r="BI50" s="118" t="n"/>
-      <c r="BJ50" s="118" t="n"/>
-      <c r="BK50" s="118" t="n"/>
-      <c r="BL50" s="118" t="n"/>
-      <c r="BM50" s="118" t="n"/>
       <c r="BN50" s="91" t="n"/>
       <c r="BO50" s="87" t="n"/>
-      <c r="BP50" s="118" t="n"/>
-      <c r="BQ50" s="118" t="n"/>
-      <c r="BR50" s="118" t="n"/>
-      <c r="BS50" s="118" t="n"/>
-      <c r="BT50" s="118" t="n"/>
-      <c r="BU50" s="118" t="n"/>
-      <c r="BV50" s="118" t="n"/>
-      <c r="BW50" s="118" t="n"/>
       <c r="BX50" s="91" t="n"/>
-      <c r="BY50" s="102" t="n"/>
-      <c r="BZ50" s="118" t="n"/>
-      <c r="CA50" s="118" t="n"/>
-      <c r="CB50" s="118" t="n"/>
-      <c r="CC50" s="118" t="n"/>
-      <c r="CD50" s="118" t="n"/>
-      <c r="CE50" s="118" t="n"/>
-      <c r="CF50" s="118" t="n"/>
-      <c r="CG50" s="118" t="n"/>
-      <c r="CH50" s="118" t="n"/>
-      <c r="CI50" s="118" t="n"/>
-      <c r="CJ50" s="118" t="n"/>
-      <c r="CK50" s="118" t="n"/>
-      <c r="CL50" s="118" t="n"/>
-      <c r="CM50" s="118" t="n"/>
-      <c r="CN50" s="118" t="n"/>
-      <c r="CO50" s="118" t="n"/>
-      <c r="CP50" s="118" t="n"/>
-      <c r="CQ50" s="143" t="n"/>
+      <c r="BY50" s="87" t="n"/>
     </row>
-    <row customHeight="1" ht="8" r="51" s="113">
+    <row customHeight="1" ht="8" r="51" s="113" spans="1:95">
       <c r="A51" s="6" t="n"/>
       <c r="B51" s="7" t="n"/>
       <c r="C51" s="7" t="n"/>
@@ -7656,40 +5262,13 @@
       <c r="S51" s="7" t="n"/>
       <c r="T51" s="7" t="n"/>
       <c r="U51" s="7" t="n"/>
-      <c r="V51" s="35" t="inlineStr">
-        <is>
-          <t>(подпись)</t>
-        </is>
-      </c>
-      <c r="W51" s="122" t="n"/>
-      <c r="X51" s="122" t="n"/>
-      <c r="Y51" s="122" t="n"/>
-      <c r="Z51" s="122" t="n"/>
-      <c r="AA51" s="122" t="n"/>
-      <c r="AB51" s="122" t="n"/>
-      <c r="AC51" s="122" t="n"/>
-      <c r="AD51" s="122" t="n"/>
-      <c r="AE51" s="122" t="n"/>
+      <c r="V51" s="35" t="s">
+        <v>67</v>
+      </c>
       <c r="AF51" s="7" t="n"/>
-      <c r="AG51" s="35" t="inlineStr">
-        <is>
-          <t>(расшифровка подписи)</t>
-        </is>
-      </c>
-      <c r="AH51" s="122" t="n"/>
-      <c r="AI51" s="122" t="n"/>
-      <c r="AJ51" s="122" t="n"/>
-      <c r="AK51" s="122" t="n"/>
-      <c r="AL51" s="122" t="n"/>
-      <c r="AM51" s="122" t="n"/>
-      <c r="AN51" s="122" t="n"/>
-      <c r="AO51" s="122" t="n"/>
-      <c r="AP51" s="122" t="n"/>
-      <c r="AQ51" s="122" t="n"/>
-      <c r="AR51" s="122" t="n"/>
-      <c r="AS51" s="122" t="n"/>
-      <c r="AT51" s="122" t="n"/>
-      <c r="AU51" s="122" t="n"/>
+      <c r="AG51" s="35" t="s">
+        <v>68</v>
+      </c>
       <c r="AV51" s="88" t="n"/>
       <c r="AW51" s="55" t="n"/>
       <c r="AX51" s="7" t="n"/>
@@ -7699,63 +5278,21 @@
       <c r="BB51" s="7" t="n"/>
       <c r="BC51" s="7" t="n"/>
       <c r="BD51" s="7" t="n"/>
-      <c r="BE51" s="35" t="inlineStr">
-        <is>
-          <t>(должность)</t>
-        </is>
-      </c>
-      <c r="BF51" s="122" t="n"/>
-      <c r="BG51" s="122" t="n"/>
-      <c r="BH51" s="122" t="n"/>
-      <c r="BI51" s="122" t="n"/>
-      <c r="BJ51" s="122" t="n"/>
-      <c r="BK51" s="122" t="n"/>
-      <c r="BL51" s="122" t="n"/>
-      <c r="BM51" s="122" t="n"/>
+      <c r="BE51" s="35" t="s">
+        <v>66</v>
+      </c>
       <c r="BN51" s="101" t="n"/>
-      <c r="BO51" s="35" t="inlineStr">
-        <is>
-          <t>(подпись)</t>
-        </is>
-      </c>
-      <c r="BP51" s="122" t="n"/>
-      <c r="BQ51" s="122" t="n"/>
-      <c r="BR51" s="122" t="n"/>
-      <c r="BS51" s="122" t="n"/>
-      <c r="BT51" s="122" t="n"/>
-      <c r="BU51" s="122" t="n"/>
-      <c r="BV51" s="122" t="n"/>
-      <c r="BW51" s="122" t="n"/>
+      <c r="BO51" s="35" t="s">
+        <v>67</v>
+      </c>
       <c r="BX51" s="101" t="n"/>
-      <c r="BY51" s="95" t="inlineStr">
-        <is>
-          <t>(расшифровка подписи)</t>
-        </is>
-      </c>
-      <c r="BZ51" s="122" t="n"/>
-      <c r="CA51" s="122" t="n"/>
-      <c r="CB51" s="122" t="n"/>
-      <c r="CC51" s="122" t="n"/>
-      <c r="CD51" s="122" t="n"/>
-      <c r="CE51" s="122" t="n"/>
-      <c r="CF51" s="122" t="n"/>
-      <c r="CG51" s="122" t="n"/>
-      <c r="CH51" s="122" t="n"/>
-      <c r="CI51" s="122" t="n"/>
-      <c r="CJ51" s="122" t="n"/>
-      <c r="CK51" s="122" t="n"/>
-      <c r="CL51" s="122" t="n"/>
-      <c r="CM51" s="122" t="n"/>
-      <c r="CN51" s="122" t="n"/>
-      <c r="CO51" s="122" t="n"/>
-      <c r="CP51" s="122" t="n"/>
-      <c r="CQ51" s="144" t="n"/>
+      <c r="BY51" s="35" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row customHeight="1" ht="14.25" r="52" s="113">
-      <c r="A52" s="86" t="inlineStr">
-        <is>
-          <t>Отпуск груза произвел</t>
-        </is>
+    <row customHeight="1" ht="14.25" r="52" s="113" spans="1:95">
+      <c r="A52" s="86" t="s">
+        <v>71</v>
       </c>
       <c r="B52" s="7" t="n"/>
       <c r="C52" s="7" t="n"/>
@@ -7768,47 +5305,14 @@
       <c r="J52" s="7" t="n"/>
       <c r="K52" s="72" t="n"/>
       <c r="L52" s="87" t="n"/>
-      <c r="M52" s="118" t="n"/>
-      <c r="N52" s="118" t="n"/>
-      <c r="O52" s="118" t="n"/>
-      <c r="P52" s="118" t="n"/>
-      <c r="Q52" s="118" t="n"/>
-      <c r="R52" s="118" t="n"/>
-      <c r="S52" s="118" t="n"/>
-      <c r="T52" s="118" t="n"/>
       <c r="U52" s="91" t="n"/>
       <c r="V52" s="87" t="n"/>
-      <c r="W52" s="118" t="n"/>
-      <c r="X52" s="118" t="n"/>
-      <c r="Y52" s="118" t="n"/>
-      <c r="Z52" s="118" t="n"/>
-      <c r="AA52" s="118" t="n"/>
-      <c r="AB52" s="118" t="n"/>
-      <c r="AC52" s="118" t="n"/>
-      <c r="AD52" s="118" t="n"/>
-      <c r="AE52" s="118" t="n"/>
       <c r="AF52" s="91" t="n"/>
       <c r="AG52" s="87" t="n"/>
-      <c r="AH52" s="118" t="n"/>
-      <c r="AI52" s="118" t="n"/>
-      <c r="AJ52" s="118" t="n"/>
-      <c r="AK52" s="118" t="n"/>
-      <c r="AL52" s="118" t="n"/>
-      <c r="AM52" s="118" t="n"/>
-      <c r="AN52" s="118" t="n"/>
-      <c r="AO52" s="118" t="n"/>
-      <c r="AP52" s="118" t="n"/>
-      <c r="AQ52" s="118" t="n"/>
-      <c r="AR52" s="118" t="n"/>
-      <c r="AS52" s="118" t="n"/>
-      <c r="AT52" s="118" t="n"/>
-      <c r="AU52" s="118" t="n"/>
       <c r="AV52" s="88" t="n"/>
       <c r="AW52" s="55" t="n"/>
-      <c r="AX52" s="72" t="inlineStr">
-        <is>
-          <t>Груз получил грузополучатель</t>
-        </is>
+      <c r="AX52" s="72" t="s">
+        <v>72</v>
       </c>
       <c r="AY52" s="7" t="n"/>
       <c r="AZ52" s="7" t="n"/>
@@ -7826,37 +5330,12 @@
       <c r="BL52" s="7" t="n"/>
       <c r="BM52" s="7" t="n"/>
       <c r="BN52" s="87" t="n"/>
-      <c r="BO52" s="118" t="n"/>
-      <c r="BP52" s="118" t="n"/>
-      <c r="BQ52" s="118" t="n"/>
-      <c r="BR52" s="118" t="n"/>
-      <c r="BS52" s="118" t="n"/>
-      <c r="BT52" s="118" t="n"/>
-      <c r="BU52" s="118" t="n"/>
-      <c r="BV52" s="118" t="n"/>
-      <c r="BW52" s="118" t="n"/>
       <c r="BX52" s="91" t="n"/>
       <c r="BY52" s="87" t="n"/>
-      <c r="BZ52" s="118" t="n"/>
-      <c r="CA52" s="118" t="n"/>
-      <c r="CB52" s="118" t="n"/>
-      <c r="CC52" s="118" t="n"/>
-      <c r="CD52" s="118" t="n"/>
       <c r="CE52" s="91" t="n"/>
-      <c r="CF52" s="102" t="n"/>
-      <c r="CG52" s="118" t="n"/>
-      <c r="CH52" s="118" t="n"/>
-      <c r="CI52" s="118" t="n"/>
-      <c r="CJ52" s="118" t="n"/>
-      <c r="CK52" s="118" t="n"/>
-      <c r="CL52" s="118" t="n"/>
-      <c r="CM52" s="118" t="n"/>
-      <c r="CN52" s="118" t="n"/>
-      <c r="CO52" s="118" t="n"/>
-      <c r="CP52" s="118" t="n"/>
-      <c r="CQ52" s="143" t="n"/>
+      <c r="CF52" s="87" t="n"/>
     </row>
-    <row customHeight="1" ht="8" r="53" s="113">
+    <row customHeight="1" ht="8" r="53" s="113" spans="1:95">
       <c r="A53" s="6" t="n"/>
       <c r="B53" s="7" t="n"/>
       <c r="C53" s="7" t="n"/>
@@ -7868,54 +5347,17 @@
       <c r="I53" s="7" t="n"/>
       <c r="J53" s="7" t="n"/>
       <c r="K53" s="7" t="n"/>
-      <c r="L53" s="35" t="inlineStr">
-        <is>
-          <t>(должность)</t>
-        </is>
-      </c>
-      <c r="M53" s="122" t="n"/>
-      <c r="N53" s="122" t="n"/>
-      <c r="O53" s="122" t="n"/>
-      <c r="P53" s="122" t="n"/>
-      <c r="Q53" s="122" t="n"/>
-      <c r="R53" s="122" t="n"/>
-      <c r="S53" s="122" t="n"/>
-      <c r="T53" s="122" t="n"/>
+      <c r="L53" s="35" t="s">
+        <v>66</v>
+      </c>
       <c r="U53" s="7" t="n"/>
-      <c r="V53" s="35" t="inlineStr">
-        <is>
-          <t>(подпись)</t>
-        </is>
-      </c>
-      <c r="W53" s="122" t="n"/>
-      <c r="X53" s="122" t="n"/>
-      <c r="Y53" s="122" t="n"/>
-      <c r="Z53" s="122" t="n"/>
-      <c r="AA53" s="122" t="n"/>
-      <c r="AB53" s="122" t="n"/>
-      <c r="AC53" s="122" t="n"/>
-      <c r="AD53" s="122" t="n"/>
-      <c r="AE53" s="122" t="n"/>
+      <c r="V53" s="35" t="s">
+        <v>67</v>
+      </c>
       <c r="AF53" s="91" t="n"/>
-      <c r="AG53" s="35" t="inlineStr">
-        <is>
-          <t>(расшифровка подписи)</t>
-        </is>
-      </c>
-      <c r="AH53" s="122" t="n"/>
-      <c r="AI53" s="122" t="n"/>
-      <c r="AJ53" s="122" t="n"/>
-      <c r="AK53" s="122" t="n"/>
-      <c r="AL53" s="122" t="n"/>
-      <c r="AM53" s="122" t="n"/>
-      <c r="AN53" s="122" t="n"/>
-      <c r="AO53" s="122" t="n"/>
-      <c r="AP53" s="122" t="n"/>
-      <c r="AQ53" s="122" t="n"/>
-      <c r="AR53" s="122" t="n"/>
-      <c r="AS53" s="122" t="n"/>
-      <c r="AT53" s="122" t="n"/>
-      <c r="AU53" s="122" t="n"/>
+      <c r="AG53" s="35" t="s">
+        <v>68</v>
+      </c>
       <c r="AV53" s="88" t="n"/>
       <c r="AW53" s="55" t="n"/>
       <c r="AX53" s="7" t="n"/>
@@ -7934,50 +5376,19 @@
       <c r="BK53" s="7" t="n"/>
       <c r="BL53" s="7" t="n"/>
       <c r="BM53" s="7" t="n"/>
-      <c r="BN53" s="35" t="inlineStr">
-        <is>
-          <t>(должность)</t>
-        </is>
-      </c>
-      <c r="BO53" s="122" t="n"/>
-      <c r="BP53" s="122" t="n"/>
-      <c r="BQ53" s="122" t="n"/>
-      <c r="BR53" s="122" t="n"/>
-      <c r="BS53" s="122" t="n"/>
-      <c r="BT53" s="122" t="n"/>
-      <c r="BU53" s="122" t="n"/>
-      <c r="BV53" s="122" t="n"/>
-      <c r="BW53" s="122" t="n"/>
+      <c r="BN53" s="35" t="s">
+        <v>66</v>
+      </c>
       <c r="BX53" s="101" t="n"/>
-      <c r="BY53" s="35" t="inlineStr">
-        <is>
-          <t>(подпись)</t>
-        </is>
-      </c>
-      <c r="BZ53" s="122" t="n"/>
-      <c r="CA53" s="122" t="n"/>
-      <c r="CB53" s="122" t="n"/>
-      <c r="CC53" s="122" t="n"/>
-      <c r="CD53" s="122" t="n"/>
+      <c r="BY53" s="35" t="s">
+        <v>67</v>
+      </c>
       <c r="CE53" s="101" t="n"/>
-      <c r="CF53" s="95" t="inlineStr">
-        <is>
-          <t>(расшифровка подписи)</t>
-        </is>
-      </c>
-      <c r="CG53" s="122" t="n"/>
-      <c r="CH53" s="122" t="n"/>
-      <c r="CI53" s="122" t="n"/>
-      <c r="CJ53" s="122" t="n"/>
-      <c r="CK53" s="122" t="n"/>
-      <c r="CL53" s="122" t="n"/>
-      <c r="CM53" s="122" t="n"/>
-      <c r="CN53" s="122" t="n"/>
-      <c r="CO53" s="122" t="n"/>
-      <c r="CP53" s="122" t="n"/>
-      <c r="CQ53" s="144" t="n"/>
+      <c r="CF53" s="35" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row customHeight="1" ht="9" r="54" s="113">
+    <row customHeight="1" ht="9" r="54" s="113" spans="1:95">
       <c r="A54" s="6" t="n"/>
       <c r="B54" s="7" t="n"/>
       <c r="C54" s="7" t="n"/>
@@ -8074,55 +5485,35 @@
       <c r="CP54" s="7" t="n"/>
       <c r="CQ54" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="55" s="113">
+    <row customHeight="1" ht="15" r="55" s="113" spans="1:95">
       <c r="A55" s="103" t="n"/>
       <c r="B55" s="104" t="n"/>
       <c r="C55" s="104" t="n"/>
       <c r="D55" s="104" t="n"/>
       <c r="E55" s="104" t="n"/>
       <c r="F55" s="104" t="n"/>
-      <c r="G55" s="105" t="inlineStr">
-        <is>
-          <t>М.П.</t>
-        </is>
+      <c r="G55" s="105" t="s">
+        <v>73</v>
       </c>
       <c r="H55" s="104" t="n"/>
       <c r="I55" s="104" t="n"/>
       <c r="J55" s="104" t="n"/>
       <c r="K55" s="104" t="n"/>
       <c r="L55" s="104" t="n"/>
-      <c r="M55" s="106" t="inlineStr">
-        <is>
-          <t>«</t>
-        </is>
+      <c r="M55" s="106" t="s">
+        <v>74</v>
       </c>
       <c r="N55" s="87" t="n"/>
-      <c r="O55" s="118" t="n"/>
-      <c r="P55" s="107" t="inlineStr">
-        <is>
-          <t>»</t>
-        </is>
+      <c r="P55" s="107" t="s">
+        <v>58</v>
       </c>
       <c r="Q55" s="104" t="n"/>
       <c r="R55" s="87" t="n"/>
-      <c r="S55" s="118" t="n"/>
-      <c r="T55" s="118" t="n"/>
-      <c r="U55" s="118" t="n"/>
-      <c r="V55" s="118" t="n"/>
-      <c r="W55" s="118" t="n"/>
-      <c r="X55" s="118" t="n"/>
-      <c r="Y55" s="118" t="n"/>
       <c r="Z55" s="107" t="n"/>
       <c r="AA55" s="87" t="n"/>
-      <c r="AB55" s="118" t="n"/>
-      <c r="AC55" s="118" t="n"/>
-      <c r="AD55" s="108" t="inlineStr">
-        <is>
-          <t>года</t>
-        </is>
-      </c>
-      <c r="AE55" s="146" t="n"/>
-      <c r="AF55" s="146" t="n"/>
+      <c r="AD55" s="108" t="s">
+        <v>75</v>
+      </c>
       <c r="AG55" s="104" t="n"/>
       <c r="AH55" s="104" t="n"/>
       <c r="AI55" s="104" t="n"/>
@@ -8140,48 +5531,28 @@
       <c r="AU55" s="104" t="n"/>
       <c r="AV55" s="109" t="n"/>
       <c r="AW55" s="110" t="n"/>
-      <c r="AX55" s="111" t="inlineStr">
-        <is>
-          <t>М.П.</t>
-        </is>
+      <c r="AX55" s="111" t="s">
+        <v>73</v>
       </c>
       <c r="AY55" s="104" t="n"/>
       <c r="AZ55" s="104" t="n"/>
       <c r="BA55" s="104" t="n"/>
       <c r="BB55" s="104" t="n"/>
       <c r="BC55" s="104" t="n"/>
-      <c r="BD55" s="106" t="inlineStr">
-        <is>
-          <t>«</t>
-        </is>
+      <c r="BD55" s="106" t="s">
+        <v>74</v>
       </c>
       <c r="BE55" s="87" t="n"/>
-      <c r="BF55" s="118" t="n"/>
-      <c r="BG55" s="107" t="inlineStr">
-        <is>
-          <t>»</t>
-        </is>
+      <c r="BG55" s="107" t="s">
+        <v>58</v>
       </c>
       <c r="BH55" s="104" t="n"/>
       <c r="BI55" s="87" t="n"/>
-      <c r="BJ55" s="118" t="n"/>
-      <c r="BK55" s="118" t="n"/>
-      <c r="BL55" s="118" t="n"/>
-      <c r="BM55" s="118" t="n"/>
-      <c r="BN55" s="118" t="n"/>
-      <c r="BO55" s="118" t="n"/>
-      <c r="BP55" s="118" t="n"/>
       <c r="BQ55" s="107" t="n"/>
       <c r="BR55" s="87" t="n"/>
-      <c r="BS55" s="118" t="n"/>
-      <c r="BT55" s="118" t="n"/>
-      <c r="BU55" s="108" t="inlineStr">
-        <is>
-          <t>года</t>
-        </is>
-      </c>
-      <c r="BV55" s="146" t="n"/>
-      <c r="BW55" s="146" t="n"/>
+      <c r="BU55" s="108" t="s">
+        <v>75</v>
+      </c>
       <c r="BX55" s="104" t="n"/>
       <c r="BY55" s="104" t="n"/>
       <c r="BZ55" s="104" t="n"/>
@@ -8204,7 +5575,7 @@
       <c r="CQ55" s="112" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="134">
+  <mergeCells count="136">
     <mergeCell ref="BU55:BW55"/>
     <mergeCell ref="BR55:BT55"/>
     <mergeCell ref="BI55:BP55"/>
@@ -8339,6 +5710,8 @@
     <mergeCell ref="CF5:CQ5"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="D31:S31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:S32"/>
   </mergeCells>
   <pageMargins bottom="0.37" footer="0.1" header="0.1" left="0.3" right="0.3" top="0.61"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" orientation="portrait" pageOrder="overThenDown" scale="100" useFirstPageNumber="0"/>

</xml_diff>